<commit_message>
Prevalence fits but there is a bug! Even 1 prob of HTN gives below 100% HTN. Check code for errors
Done:
1. Excel method files are updated, includes prevalence data overall/by age
2. File and code to 'copy' excel methods into resource files
3. Template code for risk read in

TO DO HT and Diabetes:
1. Finish updating HR as being read in
2. Set DALY to 0
3. Read in prevalence data
4. Code, print and log prevalence overall and  by age

Discuss with Tim:
1. QALY resolve (add hypertension into file?)
2. Update prevalence and incidence to fit to data (within 95% CI, with assert to fial if not)
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_HT.xlsx
+++ b/resources/ResourceFile_Method_HT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/Dropbox/Projects - ongoing/Malawi Project/Thanzi la Onse/04 - Methods Repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263DABF2-BA61-1848-BD90-EF3995834E6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425322BF-39B5-9140-9345-14B07130B04D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="26720" tabRatio="723" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16100" tabRatio="723" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -1874,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2106,7 +2106,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="38">
-        <v>0.21000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2117,7 +2117,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="38">
-        <v>0.21000000000000002</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -2128,7 +2128,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="38">
-        <v>0.21000000000000002</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2139,7 +2139,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="38">
-        <v>0.21000000000000002</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -2150,7 +2150,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="38">
-        <v>0.21000000000000002</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2161,7 +2161,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="38">
-        <v>0.21000000000000002</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -2172,7 +2172,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="38">
-        <v>0.21000000000000002</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -2183,7 +2183,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="38">
-        <v>0.21000000000000002</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2194,7 +2194,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="38">
-        <v>0.21000000000000002</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -2205,7 +2205,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="38">
-        <v>0.21000000000000002</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -2216,7 +2216,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="38">
-        <v>0.21000000000000002</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -2227,7 +2227,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="38">
-        <v>0.21000000000000002</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -2238,7 +2238,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="38">
-        <v>0.28500000000000003</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2249,7 +2249,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="38">
-        <v>0.28500000000000003</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2260,7 +2260,7 @@
         <v>32</v>
       </c>
       <c r="C34" s="38">
-        <v>0.28500000000000003</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2271,7 +2271,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="38">
-        <v>0.28500000000000003</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2282,7 +2282,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="38">
-        <v>0.28500000000000003</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2293,7 +2293,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="38">
-        <v>0.28500000000000003</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2304,7 +2304,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="38">
-        <v>0.28500000000000003</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2315,7 +2315,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="38">
-        <v>0.28500000000000003</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2326,7 +2326,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="38">
-        <v>0.28500000000000003</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2337,7 +2337,7 @@
         <v>39</v>
       </c>
       <c r="C41" s="38">
-        <v>0.28500000000000003</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2348,7 +2348,7 @@
         <v>40</v>
       </c>
       <c r="C42" s="38">
-        <v>0.44999999999999996</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2359,7 +2359,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="38">
-        <v>0.44999999999999996</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2370,7 +2370,7 @@
         <v>42</v>
       </c>
       <c r="C44" s="38">
-        <v>0.44999999999999996</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2381,7 +2381,7 @@
         <v>43</v>
       </c>
       <c r="C45" s="38">
-        <v>0.44999999999999996</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -2392,7 +2392,7 @@
         <v>44</v>
       </c>
       <c r="C46" s="38">
-        <v>0.44999999999999996</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -2403,7 +2403,7 @@
         <v>45</v>
       </c>
       <c r="C47" s="38">
-        <v>0.44999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -2414,7 +2414,7 @@
         <v>46</v>
       </c>
       <c r="C48" s="38">
-        <v>0.44999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -2425,7 +2425,7 @@
         <v>47</v>
       </c>
       <c r="C49" s="38">
-        <v>0.44999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -2436,7 +2436,7 @@
         <v>48</v>
       </c>
       <c r="C50" s="38">
-        <v>0.44999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -2447,7 +2447,7 @@
         <v>49</v>
       </c>
       <c r="C51" s="38">
-        <v>0.44999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -2458,7 +2458,7 @@
         <v>50</v>
       </c>
       <c r="C52" s="38">
-        <v>0.63</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -2469,7 +2469,7 @@
         <v>51</v>
       </c>
       <c r="C53" s="38">
-        <v>0.63</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -2480,7 +2480,7 @@
         <v>52</v>
       </c>
       <c r="C54" s="38">
-        <v>0.63</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -2491,7 +2491,7 @@
         <v>53</v>
       </c>
       <c r="C55" s="38">
-        <v>0.63</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -2502,7 +2502,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="38">
-        <v>0.63</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2513,7 +2513,7 @@
         <v>55</v>
       </c>
       <c r="C57" s="38">
-        <v>0.63</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2524,7 +2524,7 @@
         <v>56</v>
       </c>
       <c r="C58" s="38">
-        <v>0.63</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -2535,7 +2535,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="38">
-        <v>0.63</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -2546,7 +2546,7 @@
         <v>58</v>
       </c>
       <c r="C60" s="38">
-        <v>0.63</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -2557,7 +2557,7 @@
         <v>59</v>
       </c>
       <c r="C61" s="38">
-        <v>0.63</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -2568,7 +2568,7 @@
         <v>60</v>
       </c>
       <c r="C62" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -2579,7 +2579,7 @@
         <v>61</v>
       </c>
       <c r="C63" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -2590,7 +2590,7 @@
         <v>62</v>
       </c>
       <c r="C64" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -2601,7 +2601,7 @@
         <v>63</v>
       </c>
       <c r="C65" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -2612,7 +2612,7 @@
         <v>64</v>
       </c>
       <c r="C66" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -2623,7 +2623,7 @@
         <v>65</v>
       </c>
       <c r="C67" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -2634,7 +2634,7 @@
         <v>66</v>
       </c>
       <c r="C68" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -2645,7 +2645,7 @@
         <v>67</v>
       </c>
       <c r="C69" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -2656,7 +2656,7 @@
         <v>68</v>
       </c>
       <c r="C70" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -2667,7 +2667,7 @@
         <v>69</v>
       </c>
       <c r="C71" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -2678,7 +2678,7 @@
         <v>70</v>
       </c>
       <c r="C72" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -2689,7 +2689,7 @@
         <v>71</v>
       </c>
       <c r="C73" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -2700,7 +2700,7 @@
         <v>72</v>
       </c>
       <c r="C74" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -2711,7 +2711,7 @@
         <v>73</v>
       </c>
       <c r="C75" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -2722,7 +2722,7 @@
         <v>74</v>
       </c>
       <c r="C76" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -2733,7 +2733,7 @@
         <v>75</v>
       </c>
       <c r="C77" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -2744,7 +2744,7 @@
         <v>76</v>
       </c>
       <c r="C78" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -2755,7 +2755,7 @@
         <v>77</v>
       </c>
       <c r="C79" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -2766,7 +2766,7 @@
         <v>78</v>
       </c>
       <c r="C80" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -2777,7 +2777,7 @@
         <v>79</v>
       </c>
       <c r="C81" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -2788,7 +2788,7 @@
         <v>80</v>
       </c>
       <c r="C82" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -2799,7 +2799,7 @@
         <v>81</v>
       </c>
       <c r="C83" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -2810,7 +2810,7 @@
         <v>82</v>
       </c>
       <c r="C84" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -2821,7 +2821,7 @@
         <v>83</v>
       </c>
       <c r="C85" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -2832,7 +2832,7 @@
         <v>84</v>
       </c>
       <c r="C86" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -2843,7 +2843,7 @@
         <v>85</v>
       </c>
       <c r="C87" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -2854,7 +2854,7 @@
         <v>86</v>
       </c>
       <c r="C88" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -2865,7 +2865,7 @@
         <v>87</v>
       </c>
       <c r="C89" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -2876,7 +2876,7 @@
         <v>88</v>
       </c>
       <c r="C90" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -2887,7 +2887,7 @@
         <v>89</v>
       </c>
       <c r="C91" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -2898,7 +2898,7 @@
         <v>90</v>
       </c>
       <c r="C92" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -2909,7 +2909,7 @@
         <v>91</v>
       </c>
       <c r="C93" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -2920,7 +2920,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -2931,7 +2931,7 @@
         <v>93</v>
       </c>
       <c r="C95" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -2942,7 +2942,7 @@
         <v>94</v>
       </c>
       <c r="C96" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -2953,7 +2953,7 @@
         <v>95</v>
       </c>
       <c r="C97" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -2964,7 +2964,7 @@
         <v>96</v>
       </c>
       <c r="C98" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -2975,7 +2975,7 @@
         <v>97</v>
       </c>
       <c r="C99" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -2986,7 +2986,7 @@
         <v>98</v>
       </c>
       <c r="C100" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -2997,7 +2997,7 @@
         <v>99</v>
       </c>
       <c r="C101" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -3008,7 +3008,7 @@
         <v>100</v>
       </c>
       <c r="C102" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -3019,7 +3019,7 @@
         <v>101</v>
       </c>
       <c r="C103" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -3030,7 +3030,7 @@
         <v>102</v>
       </c>
       <c r="C104" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -3041,7 +3041,7 @@
         <v>103</v>
       </c>
       <c r="C105" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -3052,7 +3052,7 @@
         <v>104</v>
       </c>
       <c r="C106" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -3063,7 +3063,7 @@
         <v>105</v>
       </c>
       <c r="C107" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -3074,7 +3074,7 @@
         <v>106</v>
       </c>
       <c r="C108" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -3085,7 +3085,7 @@
         <v>107</v>
       </c>
       <c r="C109" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -3096,7 +3096,7 @@
         <v>108</v>
       </c>
       <c r="C110" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -3107,7 +3107,7 @@
         <v>109</v>
       </c>
       <c r="C111" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -3118,7 +3118,7 @@
         <v>110</v>
       </c>
       <c r="C112" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -3129,7 +3129,7 @@
         <v>111</v>
       </c>
       <c r="C113" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -3140,7 +3140,7 @@
         <v>112</v>
       </c>
       <c r="C114" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -3151,7 +3151,7 @@
         <v>113</v>
       </c>
       <c r="C115" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -3162,7 +3162,7 @@
         <v>114</v>
       </c>
       <c r="C116" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -3173,7 +3173,7 @@
         <v>115</v>
       </c>
       <c r="C117" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -3184,7 +3184,7 @@
         <v>116</v>
       </c>
       <c r="C118" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -3195,7 +3195,7 @@
         <v>117</v>
       </c>
       <c r="C119" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -3206,7 +3206,7 @@
         <v>118</v>
       </c>
       <c r="C120" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -3217,7 +3217,7 @@
         <v>119</v>
       </c>
       <c r="C121" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -3228,7 +3228,7 @@
         <v>120</v>
       </c>
       <c r="C122" s="38">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="C20" s="38">
         <f>prevalence2018!C20/100</f>
-        <v>2.1000000000000003E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3481,7 +3481,7 @@
       </c>
       <c r="C21" s="38">
         <f>prevalence2018!C21/100</f>
-        <v>2.1000000000000003E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="C22" s="38">
         <f>prevalence2018!C22/100</f>
-        <v>2.1000000000000003E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3505,7 +3505,7 @@
       </c>
       <c r="C23" s="38">
         <f>prevalence2018!C23/100</f>
-        <v>2.1000000000000003E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3517,7 +3517,7 @@
       </c>
       <c r="C24" s="38">
         <f>prevalence2018!C24/100</f>
-        <v>2.1000000000000003E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3529,7 +3529,7 @@
       </c>
       <c r="C25" s="38">
         <f>prevalence2018!C25/100</f>
-        <v>2.1000000000000003E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3541,7 +3541,7 @@
       </c>
       <c r="C26" s="38">
         <f>prevalence2018!C26/100</f>
-        <v>2.1000000000000003E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3553,7 +3553,7 @@
       </c>
       <c r="C27" s="38">
         <f>prevalence2018!C27/100</f>
-        <v>2.1000000000000003E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="C28" s="38">
         <f>prevalence2018!C28/100</f>
-        <v>2.1000000000000003E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="C29" s="38">
         <f>prevalence2018!C29/100</f>
-        <v>2.1000000000000003E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3589,7 +3589,7 @@
       </c>
       <c r="C30" s="38">
         <f>prevalence2018!C30/100</f>
-        <v>2.1000000000000003E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -3601,7 +3601,7 @@
       </c>
       <c r="C31" s="38">
         <f>prevalence2018!C31/100</f>
-        <v>2.1000000000000003E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -3613,7 +3613,7 @@
       </c>
       <c r="C32" s="38">
         <f>prevalence2018!C32/100</f>
-        <v>2.8500000000000001E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -3625,7 +3625,7 @@
       </c>
       <c r="C33" s="38">
         <f>prevalence2018!C33/100</f>
-        <v>2.8500000000000001E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -3637,7 +3637,7 @@
       </c>
       <c r="C34" s="38">
         <f>prevalence2018!C34/100</f>
-        <v>2.8500000000000001E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -3649,7 +3649,7 @@
       </c>
       <c r="C35" s="38">
         <f>prevalence2018!C35/100</f>
-        <v>2.8500000000000001E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="C36" s="38">
         <f>prevalence2018!C36/100</f>
-        <v>2.8500000000000001E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -3673,7 +3673,7 @@
       </c>
       <c r="C37" s="38">
         <f>prevalence2018!C37/100</f>
-        <v>2.8500000000000001E-3</v>
+        <v>4.3E-3</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -3685,7 +3685,7 @@
       </c>
       <c r="C38" s="38">
         <f>prevalence2018!C38/100</f>
-        <v>2.8500000000000001E-3</v>
+        <v>4.3E-3</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -3697,7 +3697,7 @@
       </c>
       <c r="C39" s="38">
         <f>prevalence2018!C39/100</f>
-        <v>2.8500000000000001E-3</v>
+        <v>4.3E-3</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -3709,7 +3709,7 @@
       </c>
       <c r="C40" s="38">
         <f>prevalence2018!C40/100</f>
-        <v>2.8500000000000001E-3</v>
+        <v>4.3E-3</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="C41" s="38">
         <f>prevalence2018!C41/100</f>
-        <v>2.8500000000000001E-3</v>
+        <v>4.3E-3</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -3733,7 +3733,7 @@
       </c>
       <c r="C42" s="38">
         <f>prevalence2018!C42/100</f>
-        <v>4.4999999999999997E-3</v>
+        <v>4.3E-3</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -3745,7 +3745,7 @@
       </c>
       <c r="C43" s="38">
         <f>prevalence2018!C43/100</f>
-        <v>4.4999999999999997E-3</v>
+        <v>4.3E-3</v>
       </c>
       <c r="I43" t="s">
         <v>60</v>
@@ -3760,7 +3760,7 @@
       </c>
       <c r="C44" s="38">
         <f>prevalence2018!C44/100</f>
-        <v>4.4999999999999997E-3</v>
+        <v>4.3E-3</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -3772,7 +3772,7 @@
       </c>
       <c r="C45" s="38">
         <f>prevalence2018!C45/100</f>
-        <v>4.4999999999999997E-3</v>
+        <v>4.3E-3</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -3784,7 +3784,7 @@
       </c>
       <c r="C46" s="38">
         <f>prevalence2018!C46/100</f>
-        <v>4.4999999999999997E-3</v>
+        <v>4.3E-3</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -3796,7 +3796,7 @@
       </c>
       <c r="C47" s="38">
         <f>prevalence2018!C47/100</f>
-        <v>4.4999999999999997E-3</v>
+        <v>5.6999999999999993E-3</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -3808,7 +3808,7 @@
       </c>
       <c r="C48" s="38">
         <f>prevalence2018!C48/100</f>
-        <v>4.4999999999999997E-3</v>
+        <v>5.6999999999999993E-3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="C49" s="38">
         <f>prevalence2018!C49/100</f>
-        <v>4.4999999999999997E-3</v>
+        <v>5.6999999999999993E-3</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -3832,7 +3832,7 @@
       </c>
       <c r="C50" s="38">
         <f>prevalence2018!C50/100</f>
-        <v>4.4999999999999997E-3</v>
+        <v>5.6999999999999993E-3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -3844,7 +3844,7 @@
       </c>
       <c r="C51" s="38">
         <f>prevalence2018!C51/100</f>
-        <v>4.4999999999999997E-3</v>
+        <v>5.6999999999999993E-3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -3856,7 +3856,7 @@
       </c>
       <c r="C52" s="38">
         <f>prevalence2018!C52/100</f>
-        <v>6.3E-3</v>
+        <v>5.6999999999999993E-3</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -3868,7 +3868,7 @@
       </c>
       <c r="C53" s="38">
         <f>prevalence2018!C53/100</f>
-        <v>6.3E-3</v>
+        <v>5.6999999999999993E-3</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -3880,7 +3880,7 @@
       </c>
       <c r="C54" s="38">
         <f>prevalence2018!C54/100</f>
-        <v>6.3E-3</v>
+        <v>5.6999999999999993E-3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -3892,7 +3892,7 @@
       </c>
       <c r="C55" s="38">
         <f>prevalence2018!C55/100</f>
-        <v>6.3E-3</v>
+        <v>5.6999999999999993E-3</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -3904,7 +3904,7 @@
       </c>
       <c r="C56" s="38">
         <f>prevalence2018!C56/100</f>
-        <v>6.3E-3</v>
+        <v>5.6999999999999993E-3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -3916,7 +3916,7 @@
       </c>
       <c r="C57" s="38">
         <f>prevalence2018!C57/100</f>
-        <v>6.3E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -3928,7 +3928,7 @@
       </c>
       <c r="C58" s="38">
         <f>prevalence2018!C58/100</f>
-        <v>6.3E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -3940,7 +3940,7 @@
       </c>
       <c r="C59" s="38">
         <f>prevalence2018!C59/100</f>
-        <v>6.3E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -3952,7 +3952,7 @@
       </c>
       <c r="C60" s="38">
         <f>prevalence2018!C60/100</f>
-        <v>6.3E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -3964,7 +3964,7 @@
       </c>
       <c r="C61" s="38">
         <f>prevalence2018!C61/100</f>
-        <v>6.3E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -3976,7 +3976,7 @@
       </c>
       <c r="C62" s="38">
         <f>prevalence2018!C62/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -3988,7 +3988,7 @@
       </c>
       <c r="C63" s="38">
         <f>prevalence2018!C63/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -4000,7 +4000,7 @@
       </c>
       <c r="C64" s="38">
         <f>prevalence2018!C64/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -4012,7 +4012,7 @@
       </c>
       <c r="C65" s="38">
         <f>prevalence2018!C65/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -4024,7 +4024,7 @@
       </c>
       <c r="C66" s="38">
         <f>prevalence2018!C66/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -4036,7 +4036,7 @@
       </c>
       <c r="C67" s="38">
         <f>prevalence2018!C67/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -4048,7 +4048,7 @@
       </c>
       <c r="C68" s="38">
         <f>prevalence2018!C68/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -4060,7 +4060,7 @@
       </c>
       <c r="C69" s="38">
         <f>prevalence2018!C69/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -4072,7 +4072,7 @@
       </c>
       <c r="C70" s="38">
         <f>prevalence2018!C70/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -4084,7 +4084,7 @@
       </c>
       <c r="C71" s="38">
         <f>prevalence2018!C71/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -4096,7 +4096,7 @@
       </c>
       <c r="C72" s="38">
         <f>prevalence2018!C72/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -4108,7 +4108,7 @@
       </c>
       <c r="C73" s="38">
         <f>prevalence2018!C73/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -4120,7 +4120,7 @@
       </c>
       <c r="C74" s="38">
         <f>prevalence2018!C74/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -4132,7 +4132,7 @@
       </c>
       <c r="C75" s="38">
         <f>prevalence2018!C75/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -4144,7 +4144,7 @@
       </c>
       <c r="C76" s="38">
         <f>prevalence2018!C76/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -4156,7 +4156,7 @@
       </c>
       <c r="C77" s="38">
         <f>prevalence2018!C77/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -4168,7 +4168,7 @@
       </c>
       <c r="C78" s="38">
         <f>prevalence2018!C78/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -4180,7 +4180,7 @@
       </c>
       <c r="C79" s="38">
         <f>prevalence2018!C79/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -4192,7 +4192,7 @@
       </c>
       <c r="C80" s="38">
         <f>prevalence2018!C80/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -4204,7 +4204,7 @@
       </c>
       <c r="C81" s="38">
         <f>prevalence2018!C81/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -4216,7 +4216,7 @@
       </c>
       <c r="C82" s="38">
         <f>prevalence2018!C82/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -4228,7 +4228,7 @@
       </c>
       <c r="C83" s="38">
         <f>prevalence2018!C83/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -4240,7 +4240,7 @@
       </c>
       <c r="C84" s="38">
         <f>prevalence2018!C84/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -4252,7 +4252,7 @@
       </c>
       <c r="C85" s="38">
         <f>prevalence2018!C85/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -4264,7 +4264,7 @@
       </c>
       <c r="C86" s="38">
         <f>prevalence2018!C86/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -4276,7 +4276,7 @@
       </c>
       <c r="C87" s="38">
         <f>prevalence2018!C87/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C88" s="38">
         <f>prevalence2018!C88/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -4300,7 +4300,7 @@
       </c>
       <c r="C89" s="38">
         <f>prevalence2018!C89/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -4312,7 +4312,7 @@
       </c>
       <c r="C90" s="38">
         <f>prevalence2018!C90/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -4324,7 +4324,7 @@
       </c>
       <c r="C91" s="38">
         <f>prevalence2018!C91/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -4336,7 +4336,7 @@
       </c>
       <c r="C92" s="38">
         <f>prevalence2018!C92/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -4348,7 +4348,7 @@
       </c>
       <c r="C93" s="38">
         <f>prevalence2018!C93/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -4360,7 +4360,7 @@
       </c>
       <c r="C94" s="38">
         <f>prevalence2018!C94/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -4372,7 +4372,7 @@
       </c>
       <c r="C95" s="38">
         <f>prevalence2018!C95/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -4384,7 +4384,7 @@
       </c>
       <c r="C96" s="38">
         <f>prevalence2018!C96/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -4396,7 +4396,7 @@
       </c>
       <c r="C97" s="38">
         <f>prevalence2018!C97/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -4408,7 +4408,7 @@
       </c>
       <c r="C98" s="38">
         <f>prevalence2018!C98/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -4420,7 +4420,7 @@
       </c>
       <c r="C99" s="38">
         <f>prevalence2018!C99/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -4432,7 +4432,7 @@
       </c>
       <c r="C100" s="38">
         <f>prevalence2018!C100/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -4444,7 +4444,7 @@
       </c>
       <c r="C101" s="38">
         <f>prevalence2018!C101/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -4456,7 +4456,7 @@
       </c>
       <c r="C102" s="38">
         <f>prevalence2018!C102/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -4468,7 +4468,7 @@
       </c>
       <c r="C103" s="38">
         <f>prevalence2018!C103/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -4480,7 +4480,7 @@
       </c>
       <c r="C104" s="38">
         <f>prevalence2018!C104/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -4492,7 +4492,7 @@
       </c>
       <c r="C105" s="38">
         <f>prevalence2018!C105/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -4504,7 +4504,7 @@
       </c>
       <c r="C106" s="38">
         <f>prevalence2018!C106/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -4516,7 +4516,7 @@
       </c>
       <c r="C107" s="38">
         <f>prevalence2018!C107/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -4528,7 +4528,7 @@
       </c>
       <c r="C108" s="38">
         <f>prevalence2018!C108/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -4540,7 +4540,7 @@
       </c>
       <c r="C109" s="38">
         <f>prevalence2018!C109/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -4552,7 +4552,7 @@
       </c>
       <c r="C110" s="38">
         <f>prevalence2018!C110/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -4564,7 +4564,7 @@
       </c>
       <c r="C111" s="38">
         <f>prevalence2018!C111/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -4576,7 +4576,7 @@
       </c>
       <c r="C112" s="38">
         <f>prevalence2018!C112/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -4588,7 +4588,7 @@
       </c>
       <c r="C113" s="38">
         <f>prevalence2018!C113/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -4600,7 +4600,7 @@
       </c>
       <c r="C114" s="38">
         <f>prevalence2018!C114/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -4612,7 +4612,7 @@
       </c>
       <c r="C115" s="38">
         <f>prevalence2018!C115/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -4624,7 +4624,7 @@
       </c>
       <c r="C116" s="38">
         <f>prevalence2018!C116/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -4636,7 +4636,7 @@
       </c>
       <c r="C117" s="38">
         <f>prevalence2018!C117/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -4648,7 +4648,7 @@
       </c>
       <c r="C118" s="38">
         <f>prevalence2018!C118/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -4660,7 +4660,7 @@
       </c>
       <c r="C119" s="38">
         <f>prevalence2018!C119/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -4672,7 +4672,7 @@
       </c>
       <c r="C120" s="38">
         <f>prevalence2018!C120/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -4684,7 +4684,7 @@
       </c>
       <c r="C121" s="38">
         <f>prevalence2018!C121/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -4696,7 +4696,7 @@
       </c>
       <c r="C122" s="38">
         <f>prevalence2018!C122/100</f>
-        <v>7.8000000000000005E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
   </sheetData>
@@ -4842,7 +4842,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7146AB7-8FEC-7F45-A5FB-E9FDE5B75DD4}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
Prevalence is now in line with STEP data.
Next steps:
1. Incidence
2. Outreach campaign
3. Treatment with triage
4. Read 95% CI for fitting?
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_HT.xlsx
+++ b/resources/ResourceFile_Method_HT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/Dropbox/Projects - ongoing/Malawi Project/Thanzi la Onse/04 - Methods Repository/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425322BF-39B5-9140-9345-14B07130B04D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547C5F82-69BB-FA4D-B38D-F8C4741650EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16100" tabRatio="723" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="26720" tabRatio="723" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1874,8 +1876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57:C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2117,7 +2119,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="38">
-        <v>0.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -2128,7 +2130,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="38">
-        <v>0.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2139,7 +2141,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="38">
-        <v>0.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -2150,7 +2152,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="38">
-        <v>0.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2161,7 +2163,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="38">
-        <v>0.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -2172,7 +2174,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="38">
-        <v>0.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -2183,7 +2185,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="38">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2194,7 +2196,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="38">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -2205,7 +2207,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="38">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -2216,7 +2218,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="38">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -2227,7 +2229,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="38">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -2238,7 +2240,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="38">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2249,7 +2251,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="38">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2260,7 +2262,7 @@
         <v>32</v>
       </c>
       <c r="C34" s="38">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2271,7 +2273,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="38">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2282,7 +2284,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="38">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2293,7 +2295,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="38">
-        <v>0.43</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2304,7 +2306,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="38">
-        <v>0.43</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2315,7 +2317,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="38">
-        <v>0.43</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2326,7 +2328,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="38">
-        <v>0.43</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2337,7 +2339,7 @@
         <v>39</v>
       </c>
       <c r="C41" s="38">
-        <v>0.43</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2348,7 +2350,7 @@
         <v>40</v>
       </c>
       <c r="C42" s="38">
-        <v>0.43</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2359,7 +2361,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="38">
-        <v>0.43</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2370,7 +2372,7 @@
         <v>42</v>
       </c>
       <c r="C44" s="38">
-        <v>0.43</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2381,7 +2383,7 @@
         <v>43</v>
       </c>
       <c r="C45" s="38">
-        <v>0.43</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -2392,7 +2394,7 @@
         <v>44</v>
       </c>
       <c r="C46" s="38">
-        <v>0.43</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -2403,7 +2405,7 @@
         <v>45</v>
       </c>
       <c r="C47" s="38">
-        <v>0.56999999999999995</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -2414,7 +2416,7 @@
         <v>46</v>
       </c>
       <c r="C48" s="38">
-        <v>0.56999999999999995</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -2425,7 +2427,7 @@
         <v>47</v>
       </c>
       <c r="C49" s="38">
-        <v>0.56999999999999995</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -2436,7 +2438,7 @@
         <v>48</v>
       </c>
       <c r="C50" s="38">
-        <v>0.56999999999999995</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -2447,7 +2449,7 @@
         <v>49</v>
       </c>
       <c r="C51" s="38">
-        <v>0.56999999999999995</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -2458,7 +2460,7 @@
         <v>50</v>
       </c>
       <c r="C52" s="38">
-        <v>0.56999999999999995</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -2469,7 +2471,7 @@
         <v>51</v>
       </c>
       <c r="C53" s="38">
-        <v>0.56999999999999995</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -2480,7 +2482,7 @@
         <v>52</v>
       </c>
       <c r="C54" s="38">
-        <v>0.56999999999999995</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -2491,7 +2493,7 @@
         <v>53</v>
       </c>
       <c r="C55" s="38">
-        <v>0.56999999999999995</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -2502,7 +2504,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="38">
-        <v>0.56999999999999995</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2513,7 +2515,7 @@
         <v>55</v>
       </c>
       <c r="C57" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2524,7 +2526,7 @@
         <v>56</v>
       </c>
       <c r="C58" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -2535,7 +2537,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -2546,7 +2548,7 @@
         <v>58</v>
       </c>
       <c r="C60" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -2557,7 +2559,7 @@
         <v>59</v>
       </c>
       <c r="C61" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -2568,7 +2570,7 @@
         <v>60</v>
       </c>
       <c r="C62" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -2579,7 +2581,7 @@
         <v>61</v>
       </c>
       <c r="C63" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -2590,7 +2592,7 @@
         <v>62</v>
       </c>
       <c r="C64" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -2601,7 +2603,7 @@
         <v>63</v>
       </c>
       <c r="C65" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -2612,7 +2614,7 @@
         <v>64</v>
       </c>
       <c r="C66" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -2623,7 +2625,7 @@
         <v>65</v>
       </c>
       <c r="C67" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -2634,7 +2636,7 @@
         <v>66</v>
       </c>
       <c r="C68" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -2645,7 +2647,7 @@
         <v>67</v>
       </c>
       <c r="C69" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -2656,7 +2658,7 @@
         <v>68</v>
       </c>
       <c r="C70" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -2667,7 +2669,7 @@
         <v>69</v>
       </c>
       <c r="C71" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -2678,7 +2680,7 @@
         <v>70</v>
       </c>
       <c r="C72" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -2689,7 +2691,7 @@
         <v>71</v>
       </c>
       <c r="C73" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -2700,7 +2702,7 @@
         <v>72</v>
       </c>
       <c r="C74" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -2711,7 +2713,7 @@
         <v>73</v>
       </c>
       <c r="C75" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -2722,7 +2724,7 @@
         <v>74</v>
       </c>
       <c r="C76" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -2733,7 +2735,7 @@
         <v>75</v>
       </c>
       <c r="C77" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -2744,7 +2746,7 @@
         <v>76</v>
       </c>
       <c r="C78" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -2755,7 +2757,7 @@
         <v>77</v>
       </c>
       <c r="C79" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -2766,7 +2768,7 @@
         <v>78</v>
       </c>
       <c r="C80" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -2777,7 +2779,7 @@
         <v>79</v>
       </c>
       <c r="C81" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -2788,7 +2790,7 @@
         <v>80</v>
       </c>
       <c r="C82" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -2799,7 +2801,7 @@
         <v>81</v>
       </c>
       <c r="C83" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -2810,7 +2812,7 @@
         <v>82</v>
       </c>
       <c r="C84" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -2821,7 +2823,7 @@
         <v>83</v>
       </c>
       <c r="C85" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -2832,7 +2834,7 @@
         <v>84</v>
       </c>
       <c r="C86" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -2843,7 +2845,7 @@
         <v>85</v>
       </c>
       <c r="C87" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -2854,7 +2856,7 @@
         <v>86</v>
       </c>
       <c r="C88" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -2865,7 +2867,7 @@
         <v>87</v>
       </c>
       <c r="C89" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -2876,7 +2878,7 @@
         <v>88</v>
       </c>
       <c r="C90" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -2887,7 +2889,7 @@
         <v>89</v>
       </c>
       <c r="C91" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -2898,7 +2900,7 @@
         <v>90</v>
       </c>
       <c r="C92" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -2909,7 +2911,7 @@
         <v>91</v>
       </c>
       <c r="C93" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -2920,7 +2922,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -2931,7 +2933,7 @@
         <v>93</v>
       </c>
       <c r="C95" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -2942,7 +2944,7 @@
         <v>94</v>
       </c>
       <c r="C96" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -2953,7 +2955,7 @@
         <v>95</v>
       </c>
       <c r="C97" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -2964,7 +2966,7 @@
         <v>96</v>
       </c>
       <c r="C98" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -2975,7 +2977,7 @@
         <v>97</v>
       </c>
       <c r="C99" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -2986,7 +2988,7 @@
         <v>98</v>
       </c>
       <c r="C100" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -2997,7 +2999,7 @@
         <v>99</v>
       </c>
       <c r="C101" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -3008,7 +3010,7 @@
         <v>100</v>
       </c>
       <c r="C102" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -3019,7 +3021,7 @@
         <v>101</v>
       </c>
       <c r="C103" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -3030,7 +3032,7 @@
         <v>102</v>
       </c>
       <c r="C104" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -3041,7 +3043,7 @@
         <v>103</v>
       </c>
       <c r="C105" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -3052,7 +3054,7 @@
         <v>104</v>
       </c>
       <c r="C106" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -3063,7 +3065,7 @@
         <v>105</v>
       </c>
       <c r="C107" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -3074,7 +3076,7 @@
         <v>106</v>
       </c>
       <c r="C108" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -3085,7 +3087,7 @@
         <v>107</v>
       </c>
       <c r="C109" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -3096,7 +3098,7 @@
         <v>108</v>
       </c>
       <c r="C110" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -3107,7 +3109,7 @@
         <v>109</v>
       </c>
       <c r="C111" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -3118,7 +3120,7 @@
         <v>110</v>
       </c>
       <c r="C112" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -3129,7 +3131,7 @@
         <v>111</v>
       </c>
       <c r="C113" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -3140,7 +3142,7 @@
         <v>112</v>
       </c>
       <c r="C114" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -3151,7 +3153,7 @@
         <v>113</v>
       </c>
       <c r="C115" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -3162,7 +3164,7 @@
         <v>114</v>
       </c>
       <c r="C116" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -3173,7 +3175,7 @@
         <v>115</v>
       </c>
       <c r="C117" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -3184,7 +3186,7 @@
         <v>116</v>
       </c>
       <c r="C118" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -3195,7 +3197,7 @@
         <v>117</v>
       </c>
       <c r="C119" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -3206,7 +3208,7 @@
         <v>118</v>
       </c>
       <c r="C120" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -3217,7 +3219,7 @@
         <v>119</v>
       </c>
       <c r="C121" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -3228,7 +3230,7 @@
         <v>120</v>
       </c>
       <c r="C122" s="38">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
     </row>
   </sheetData>
@@ -3481,7 +3483,7 @@
       </c>
       <c r="C21" s="38">
         <f>prevalence2018!C21/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3493,7 +3495,7 @@
       </c>
       <c r="C22" s="38">
         <f>prevalence2018!C22/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3505,7 +3507,7 @@
       </c>
       <c r="C23" s="38">
         <f>prevalence2018!C23/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3517,7 +3519,7 @@
       </c>
       <c r="C24" s="38">
         <f>prevalence2018!C24/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3529,7 +3531,7 @@
       </c>
       <c r="C25" s="38">
         <f>prevalence2018!C25/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3541,7 +3543,7 @@
       </c>
       <c r="C26" s="38">
         <f>prevalence2018!C26/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3553,7 +3555,7 @@
       </c>
       <c r="C27" s="38">
         <f>prevalence2018!C27/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3565,7 +3567,7 @@
       </c>
       <c r="C28" s="38">
         <f>prevalence2018!C28/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3577,7 +3579,7 @@
       </c>
       <c r="C29" s="38">
         <f>prevalence2018!C29/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3589,7 +3591,7 @@
       </c>
       <c r="C30" s="38">
         <f>prevalence2018!C30/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -3601,7 +3603,7 @@
       </c>
       <c r="C31" s="38">
         <f>prevalence2018!C31/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -3613,7 +3615,7 @@
       </c>
       <c r="C32" s="38">
         <f>prevalence2018!C32/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -3625,7 +3627,7 @@
       </c>
       <c r="C33" s="38">
         <f>prevalence2018!C33/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -3637,7 +3639,7 @@
       </c>
       <c r="C34" s="38">
         <f>prevalence2018!C34/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -3649,7 +3651,7 @@
       </c>
       <c r="C35" s="38">
         <f>prevalence2018!C35/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -3661,7 +3663,7 @@
       </c>
       <c r="C36" s="38">
         <f>prevalence2018!C36/100</f>
-        <v>3.4999999999999996E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -3673,7 +3675,7 @@
       </c>
       <c r="C37" s="38">
         <f>prevalence2018!C37/100</f>
-        <v>4.3E-3</v>
+        <v>4.2500000000000003E-3</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -3685,7 +3687,7 @@
       </c>
       <c r="C38" s="38">
         <f>prevalence2018!C38/100</f>
-        <v>4.3E-3</v>
+        <v>4.2500000000000003E-3</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -3697,7 +3699,7 @@
       </c>
       <c r="C39" s="38">
         <f>prevalence2018!C39/100</f>
-        <v>4.3E-3</v>
+        <v>4.2500000000000003E-3</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -3709,7 +3711,7 @@
       </c>
       <c r="C40" s="38">
         <f>prevalence2018!C40/100</f>
-        <v>4.3E-3</v>
+        <v>4.2500000000000003E-3</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -3721,7 +3723,7 @@
       </c>
       <c r="C41" s="38">
         <f>prevalence2018!C41/100</f>
-        <v>4.3E-3</v>
+        <v>4.2500000000000003E-3</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -3733,7 +3735,7 @@
       </c>
       <c r="C42" s="38">
         <f>prevalence2018!C42/100</f>
-        <v>4.3E-3</v>
+        <v>4.2500000000000003E-3</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -3745,7 +3747,7 @@
       </c>
       <c r="C43" s="38">
         <f>prevalence2018!C43/100</f>
-        <v>4.3E-3</v>
+        <v>4.2500000000000003E-3</v>
       </c>
       <c r="I43" t="s">
         <v>60</v>
@@ -3760,7 +3762,7 @@
       </c>
       <c r="C44" s="38">
         <f>prevalence2018!C44/100</f>
-        <v>4.3E-3</v>
+        <v>4.2500000000000003E-3</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -3772,7 +3774,7 @@
       </c>
       <c r="C45" s="38">
         <f>prevalence2018!C45/100</f>
-        <v>4.3E-3</v>
+        <v>4.2500000000000003E-3</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -3784,7 +3786,7 @@
       </c>
       <c r="C46" s="38">
         <f>prevalence2018!C46/100</f>
-        <v>4.3E-3</v>
+        <v>4.2500000000000003E-3</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -3796,7 +3798,7 @@
       </c>
       <c r="C47" s="38">
         <f>prevalence2018!C47/100</f>
-        <v>5.6999999999999993E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -3808,7 +3810,7 @@
       </c>
       <c r="C48" s="38">
         <f>prevalence2018!C48/100</f>
-        <v>5.6999999999999993E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -3820,7 +3822,7 @@
       </c>
       <c r="C49" s="38">
         <f>prevalence2018!C49/100</f>
-        <v>5.6999999999999993E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -3832,7 +3834,7 @@
       </c>
       <c r="C50" s="38">
         <f>prevalence2018!C50/100</f>
-        <v>5.6999999999999993E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -3844,7 +3846,7 @@
       </c>
       <c r="C51" s="38">
         <f>prevalence2018!C51/100</f>
-        <v>5.6999999999999993E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -3856,7 +3858,7 @@
       </c>
       <c r="C52" s="38">
         <f>prevalence2018!C52/100</f>
-        <v>5.6999999999999993E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -3868,7 +3870,7 @@
       </c>
       <c r="C53" s="38">
         <f>prevalence2018!C53/100</f>
-        <v>5.6999999999999993E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -3880,7 +3882,7 @@
       </c>
       <c r="C54" s="38">
         <f>prevalence2018!C54/100</f>
-        <v>5.6999999999999993E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -3892,7 +3894,7 @@
       </c>
       <c r="C55" s="38">
         <f>prevalence2018!C55/100</f>
-        <v>5.6999999999999993E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -3904,7 +3906,7 @@
       </c>
       <c r="C56" s="38">
         <f>prevalence2018!C56/100</f>
-        <v>5.6999999999999993E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -3916,7 +3918,7 @@
       </c>
       <c r="C57" s="38">
         <f>prevalence2018!C57/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -3928,7 +3930,7 @@
       </c>
       <c r="C58" s="38">
         <f>prevalence2018!C58/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -3940,7 +3942,7 @@
       </c>
       <c r="C59" s="38">
         <f>prevalence2018!C59/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -3952,7 +3954,7 @@
       </c>
       <c r="C60" s="38">
         <f>prevalence2018!C60/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -3964,7 +3966,7 @@
       </c>
       <c r="C61" s="38">
         <f>prevalence2018!C61/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -3976,7 +3978,7 @@
       </c>
       <c r="C62" s="38">
         <f>prevalence2018!C62/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -3988,7 +3990,7 @@
       </c>
       <c r="C63" s="38">
         <f>prevalence2018!C63/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -4000,7 +4002,7 @@
       </c>
       <c r="C64" s="38">
         <f>prevalence2018!C64/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -4012,7 +4014,7 @@
       </c>
       <c r="C65" s="38">
         <f>prevalence2018!C65/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -4024,7 +4026,7 @@
       </c>
       <c r="C66" s="38">
         <f>prevalence2018!C66/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -4036,7 +4038,7 @@
       </c>
       <c r="C67" s="38">
         <f>prevalence2018!C67/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -4048,7 +4050,7 @@
       </c>
       <c r="C68" s="38">
         <f>prevalence2018!C68/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -4060,7 +4062,7 @@
       </c>
       <c r="C69" s="38">
         <f>prevalence2018!C69/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -4072,7 +4074,7 @@
       </c>
       <c r="C70" s="38">
         <f>prevalence2018!C70/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -4084,7 +4086,7 @@
       </c>
       <c r="C71" s="38">
         <f>prevalence2018!C71/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -4096,7 +4098,7 @@
       </c>
       <c r="C72" s="38">
         <f>prevalence2018!C72/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -4108,7 +4110,7 @@
       </c>
       <c r="C73" s="38">
         <f>prevalence2018!C73/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -4120,7 +4122,7 @@
       </c>
       <c r="C74" s="38">
         <f>prevalence2018!C74/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -4132,7 +4134,7 @@
       </c>
       <c r="C75" s="38">
         <f>prevalence2018!C75/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -4144,7 +4146,7 @@
       </c>
       <c r="C76" s="38">
         <f>prevalence2018!C76/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -4156,7 +4158,7 @@
       </c>
       <c r="C77" s="38">
         <f>prevalence2018!C77/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -4168,7 +4170,7 @@
       </c>
       <c r="C78" s="38">
         <f>prevalence2018!C78/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -4180,7 +4182,7 @@
       </c>
       <c r="C79" s="38">
         <f>prevalence2018!C79/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -4192,7 +4194,7 @@
       </c>
       <c r="C80" s="38">
         <f>prevalence2018!C80/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -4204,7 +4206,7 @@
       </c>
       <c r="C81" s="38">
         <f>prevalence2018!C81/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -4216,7 +4218,7 @@
       </c>
       <c r="C82" s="38">
         <f>prevalence2018!C82/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -4228,7 +4230,7 @@
       </c>
       <c r="C83" s="38">
         <f>prevalence2018!C83/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -4240,7 +4242,7 @@
       </c>
       <c r="C84" s="38">
         <f>prevalence2018!C84/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -4252,7 +4254,7 @@
       </c>
       <c r="C85" s="38">
         <f>prevalence2018!C85/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -4264,7 +4266,7 @@
       </c>
       <c r="C86" s="38">
         <f>prevalence2018!C86/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -4276,7 +4278,7 @@
       </c>
       <c r="C87" s="38">
         <f>prevalence2018!C87/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -4288,7 +4290,7 @@
       </c>
       <c r="C88" s="38">
         <f>prevalence2018!C88/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -4300,7 +4302,7 @@
       </c>
       <c r="C89" s="38">
         <f>prevalence2018!C89/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -4312,7 +4314,7 @@
       </c>
       <c r="C90" s="38">
         <f>prevalence2018!C90/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -4324,7 +4326,7 @@
       </c>
       <c r="C91" s="38">
         <f>prevalence2018!C91/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -4336,7 +4338,7 @@
       </c>
       <c r="C92" s="38">
         <f>prevalence2018!C92/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -4348,7 +4350,7 @@
       </c>
       <c r="C93" s="38">
         <f>prevalence2018!C93/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -4360,7 +4362,7 @@
       </c>
       <c r="C94" s="38">
         <f>prevalence2018!C94/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -4372,7 +4374,7 @@
       </c>
       <c r="C95" s="38">
         <f>prevalence2018!C95/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -4384,7 +4386,7 @@
       </c>
       <c r="C96" s="38">
         <f>prevalence2018!C96/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -4396,7 +4398,7 @@
       </c>
       <c r="C97" s="38">
         <f>prevalence2018!C97/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -4408,7 +4410,7 @@
       </c>
       <c r="C98" s="38">
         <f>prevalence2018!C98/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -4420,7 +4422,7 @@
       </c>
       <c r="C99" s="38">
         <f>prevalence2018!C99/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -4432,7 +4434,7 @@
       </c>
       <c r="C100" s="38">
         <f>prevalence2018!C100/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -4444,7 +4446,7 @@
       </c>
       <c r="C101" s="38">
         <f>prevalence2018!C101/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -4456,7 +4458,7 @@
       </c>
       <c r="C102" s="38">
         <f>prevalence2018!C102/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -4468,7 +4470,7 @@
       </c>
       <c r="C103" s="38">
         <f>prevalence2018!C103/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -4480,7 +4482,7 @@
       </c>
       <c r="C104" s="38">
         <f>prevalence2018!C104/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -4492,7 +4494,7 @@
       </c>
       <c r="C105" s="38">
         <f>prevalence2018!C105/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -4504,7 +4506,7 @@
       </c>
       <c r="C106" s="38">
         <f>prevalence2018!C106/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -4516,7 +4518,7 @@
       </c>
       <c r="C107" s="38">
         <f>prevalence2018!C107/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -4528,7 +4530,7 @@
       </c>
       <c r="C108" s="38">
         <f>prevalence2018!C108/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -4540,7 +4542,7 @@
       </c>
       <c r="C109" s="38">
         <f>prevalence2018!C109/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -4552,7 +4554,7 @@
       </c>
       <c r="C110" s="38">
         <f>prevalence2018!C110/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -4564,7 +4566,7 @@
       </c>
       <c r="C111" s="38">
         <f>prevalence2018!C111/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -4576,7 +4578,7 @@
       </c>
       <c r="C112" s="38">
         <f>prevalence2018!C112/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -4588,7 +4590,7 @@
       </c>
       <c r="C113" s="38">
         <f>prevalence2018!C113/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -4600,7 +4602,7 @@
       </c>
       <c r="C114" s="38">
         <f>prevalence2018!C114/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -4612,7 +4614,7 @@
       </c>
       <c r="C115" s="38">
         <f>prevalence2018!C115/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -4624,7 +4626,7 @@
       </c>
       <c r="C116" s="38">
         <f>prevalence2018!C116/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -4636,7 +4638,7 @@
       </c>
       <c r="C117" s="38">
         <f>prevalence2018!C117/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -4648,7 +4650,7 @@
       </c>
       <c r="C118" s="38">
         <f>prevalence2018!C118/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -4660,7 +4662,7 @@
       </c>
       <c r="C119" s="38">
         <f>prevalence2018!C119/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -4672,7 +4674,7 @@
       </c>
       <c r="C120" s="38">
         <f>prevalence2018!C120/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -4684,7 +4686,7 @@
       </c>
       <c r="C121" s="38">
         <f>prevalence2018!C121/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -4696,7 +4698,7 @@
       </c>
       <c r="C122" s="38">
         <f>prevalence2018!C122/100</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
   </sheetData>
@@ -4843,7 +4845,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D5" sqref="D5:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Ready to fit incidence. OK but not perfect.
To fix:
1. Log and plot
2. Read in 95% CI for plot
3. Trial outreach campaign
4. HSI event not running
5. Treatment with triage
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_HT.xlsx
+++ b/resources/ResourceFile_Method_HT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547C5F82-69BB-FA4D-B38D-F8C4741650EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165FC138-1063-B64C-98F0-69418B7623A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="26720" tabRatio="723" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34140" yWindow="460" windowWidth="17060" windowHeight="26720" tabRatio="723" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -1876,8 +1876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57:C122"/>
+    <sheetView topLeftCell="A18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3243,8 +3243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3554,8 +3554,8 @@
         <v>25</v>
       </c>
       <c r="C27" s="38">
-        <f>prevalence2018!C27/100</f>
-        <v>3.5999999999999999E-3</v>
+        <f>prevalence2018!C27/2</f>
+        <v>0.18</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3566,8 +3566,8 @@
         <v>26</v>
       </c>
       <c r="C28" s="38">
-        <f>prevalence2018!C28/100</f>
-        <v>3.5999999999999999E-3</v>
+        <f>prevalence2018!C28/2</f>
+        <v>0.18</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3578,8 +3578,8 @@
         <v>27</v>
       </c>
       <c r="C29" s="38">
-        <f>prevalence2018!C29/100</f>
-        <v>3.5999999999999999E-3</v>
+        <f>prevalence2018!C29/2</f>
+        <v>0.18</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3590,8 +3590,8 @@
         <v>28</v>
       </c>
       <c r="C30" s="38">
-        <f>prevalence2018!C30/100</f>
-        <v>3.5999999999999999E-3</v>
+        <f>prevalence2018!C30/2</f>
+        <v>0.18</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -3602,8 +3602,8 @@
         <v>29</v>
       </c>
       <c r="C31" s="38">
-        <f>prevalence2018!C31/100</f>
-        <v>3.5999999999999999E-3</v>
+        <f>prevalence2018!C31/2</f>
+        <v>0.18</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -3614,8 +3614,8 @@
         <v>30</v>
       </c>
       <c r="C32" s="38">
-        <f>prevalence2018!C32/100</f>
-        <v>3.5999999999999999E-3</v>
+        <f>prevalence2018!C32/2</f>
+        <v>0.18</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -3626,8 +3626,8 @@
         <v>31</v>
       </c>
       <c r="C33" s="38">
-        <f>prevalence2018!C33/100</f>
-        <v>3.5999999999999999E-3</v>
+        <f>prevalence2018!C33/2</f>
+        <v>0.18</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -3638,8 +3638,8 @@
         <v>32</v>
       </c>
       <c r="C34" s="38">
-        <f>prevalence2018!C34/100</f>
-        <v>3.5999999999999999E-3</v>
+        <f>prevalence2018!C34/2</f>
+        <v>0.18</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -3650,8 +3650,8 @@
         <v>33</v>
       </c>
       <c r="C35" s="38">
-        <f>prevalence2018!C35/100</f>
-        <v>3.5999999999999999E-3</v>
+        <f>prevalence2018!C35/2</f>
+        <v>0.18</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -3662,8 +3662,8 @@
         <v>34</v>
       </c>
       <c r="C36" s="38">
-        <f>prevalence2018!C36/100</f>
-        <v>3.5999999999999999E-3</v>
+        <f>prevalence2018!C36/2</f>
+        <v>0.18</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -3674,8 +3674,8 @@
         <v>35</v>
       </c>
       <c r="C37" s="38">
-        <f>prevalence2018!C37/100</f>
-        <v>4.2500000000000003E-3</v>
+        <f>prevalence2018!C37/2</f>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -3686,8 +3686,8 @@
         <v>36</v>
       </c>
       <c r="C38" s="38">
-        <f>prevalence2018!C38/100</f>
-        <v>4.2500000000000003E-3</v>
+        <f>prevalence2018!C38/2</f>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -3698,8 +3698,8 @@
         <v>37</v>
       </c>
       <c r="C39" s="38">
-        <f>prevalence2018!C39/100</f>
-        <v>4.2500000000000003E-3</v>
+        <f>prevalence2018!C39/2</f>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -3710,8 +3710,8 @@
         <v>38</v>
       </c>
       <c r="C40" s="38">
-        <f>prevalence2018!C40/100</f>
-        <v>4.2500000000000003E-3</v>
+        <f>prevalence2018!C40/2</f>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -3722,8 +3722,8 @@
         <v>39</v>
       </c>
       <c r="C41" s="38">
-        <f>prevalence2018!C41/100</f>
-        <v>4.2500000000000003E-3</v>
+        <f>prevalence2018!C41/2</f>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -3734,8 +3734,8 @@
         <v>40</v>
       </c>
       <c r="C42" s="38">
-        <f>prevalence2018!C42/100</f>
-        <v>4.2500000000000003E-3</v>
+        <f>prevalence2018!C42/2</f>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -3746,8 +3746,8 @@
         <v>41</v>
       </c>
       <c r="C43" s="38">
-        <f>prevalence2018!C43/100</f>
-        <v>4.2500000000000003E-3</v>
+        <f>prevalence2018!C43/2</f>
+        <v>0.21249999999999999</v>
       </c>
       <c r="I43" t="s">
         <v>60</v>
@@ -3761,8 +3761,8 @@
         <v>42</v>
       </c>
       <c r="C44" s="38">
-        <f>prevalence2018!C44/100</f>
-        <v>4.2500000000000003E-3</v>
+        <f>prevalence2018!C44/2</f>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -3773,8 +3773,8 @@
         <v>43</v>
       </c>
       <c r="C45" s="38">
-        <f>prevalence2018!C45/100</f>
-        <v>4.2500000000000003E-3</v>
+        <f>prevalence2018!C45/2</f>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -3785,8 +3785,8 @@
         <v>44</v>
       </c>
       <c r="C46" s="38">
-        <f>prevalence2018!C46/100</f>
-        <v>4.2500000000000003E-3</v>
+        <f>prevalence2018!C46/2</f>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -3797,8 +3797,8 @@
         <v>45</v>
       </c>
       <c r="C47" s="38">
-        <f>prevalence2018!C47/100</f>
-        <v>5.0000000000000001E-3</v>
+        <f>prevalence2018!C47/2</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -3809,8 +3809,8 @@
         <v>46</v>
       </c>
       <c r="C48" s="38">
-        <f>prevalence2018!C48/100</f>
-        <v>5.0000000000000001E-3</v>
+        <f>prevalence2018!C48/2</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -3821,8 +3821,8 @@
         <v>47</v>
       </c>
       <c r="C49" s="38">
-        <f>prevalence2018!C49/100</f>
-        <v>5.0000000000000001E-3</v>
+        <f>prevalence2018!C49/2</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -3833,8 +3833,8 @@
         <v>48</v>
       </c>
       <c r="C50" s="38">
-        <f>prevalence2018!C50/100</f>
-        <v>5.0000000000000001E-3</v>
+        <f>prevalence2018!C50/2</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -3845,8 +3845,8 @@
         <v>49</v>
       </c>
       <c r="C51" s="38">
-        <f>prevalence2018!C51/100</f>
-        <v>5.0000000000000001E-3</v>
+        <f>prevalence2018!C51/2</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -3857,8 +3857,8 @@
         <v>50</v>
       </c>
       <c r="C52" s="38">
-        <f>prevalence2018!C52/100</f>
-        <v>5.0000000000000001E-3</v>
+        <f>prevalence2018!C52/2</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -3869,8 +3869,8 @@
         <v>51</v>
       </c>
       <c r="C53" s="38">
-        <f>prevalence2018!C53/100</f>
-        <v>5.0000000000000001E-3</v>
+        <f>prevalence2018!C53/2</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -3881,8 +3881,8 @@
         <v>52</v>
       </c>
       <c r="C54" s="38">
-        <f>prevalence2018!C54/100</f>
-        <v>5.0000000000000001E-3</v>
+        <f>prevalence2018!C54/2</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -3893,8 +3893,8 @@
         <v>53</v>
       </c>
       <c r="C55" s="38">
-        <f>prevalence2018!C55/100</f>
-        <v>5.0000000000000001E-3</v>
+        <f>prevalence2018!C55/2</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -3905,8 +3905,8 @@
         <v>54</v>
       </c>
       <c r="C56" s="38">
-        <f>prevalence2018!C56/100</f>
-        <v>5.0000000000000001E-3</v>
+        <f>prevalence2018!C56/2</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -3917,8 +3917,8 @@
         <v>55</v>
       </c>
       <c r="C57" s="38">
-        <f>prevalence2018!C57/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C57/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -3929,8 +3929,8 @@
         <v>56</v>
       </c>
       <c r="C58" s="38">
-        <f>prevalence2018!C58/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C58/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -3941,8 +3941,8 @@
         <v>57</v>
       </c>
       <c r="C59" s="38">
-        <f>prevalence2018!C59/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C59/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -3953,8 +3953,8 @@
         <v>58</v>
       </c>
       <c r="C60" s="38">
-        <f>prevalence2018!C60/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C60/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -3965,8 +3965,8 @@
         <v>59</v>
       </c>
       <c r="C61" s="38">
-        <f>prevalence2018!C61/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C61/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -3977,8 +3977,8 @@
         <v>60</v>
       </c>
       <c r="C62" s="38">
-        <f>prevalence2018!C62/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C62/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -3989,8 +3989,8 @@
         <v>61</v>
       </c>
       <c r="C63" s="38">
-        <f>prevalence2018!C63/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C63/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -4001,8 +4001,8 @@
         <v>62</v>
       </c>
       <c r="C64" s="38">
-        <f>prevalence2018!C64/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C64/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -4013,8 +4013,8 @@
         <v>63</v>
       </c>
       <c r="C65" s="38">
-        <f>prevalence2018!C65/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C65/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -4025,8 +4025,8 @@
         <v>64</v>
       </c>
       <c r="C66" s="38">
-        <f>prevalence2018!C66/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C66/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -4037,8 +4037,8 @@
         <v>65</v>
       </c>
       <c r="C67" s="38">
-        <f>prevalence2018!C67/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C67/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -4049,8 +4049,8 @@
         <v>66</v>
       </c>
       <c r="C68" s="38">
-        <f>prevalence2018!C68/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C68/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -4061,8 +4061,8 @@
         <v>67</v>
       </c>
       <c r="C69" s="38">
-        <f>prevalence2018!C69/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C69/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -4073,8 +4073,8 @@
         <v>68</v>
       </c>
       <c r="C70" s="38">
-        <f>prevalence2018!C70/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C70/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -4085,8 +4085,8 @@
         <v>69</v>
       </c>
       <c r="C71" s="38">
-        <f>prevalence2018!C71/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C71/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -4097,8 +4097,8 @@
         <v>70</v>
       </c>
       <c r="C72" s="38">
-        <f>prevalence2018!C72/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C72/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -4109,8 +4109,8 @@
         <v>71</v>
       </c>
       <c r="C73" s="38">
-        <f>prevalence2018!C73/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C73/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -4121,8 +4121,8 @@
         <v>72</v>
       </c>
       <c r="C74" s="38">
-        <f>prevalence2018!C74/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C74/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -4133,8 +4133,8 @@
         <v>73</v>
       </c>
       <c r="C75" s="38">
-        <f>prevalence2018!C75/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C75/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -4145,8 +4145,8 @@
         <v>74</v>
       </c>
       <c r="C76" s="38">
-        <f>prevalence2018!C76/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C76/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -4157,8 +4157,8 @@
         <v>75</v>
       </c>
       <c r="C77" s="38">
-        <f>prevalence2018!C77/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C77/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -4169,8 +4169,8 @@
         <v>76</v>
       </c>
       <c r="C78" s="38">
-        <f>prevalence2018!C78/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C78/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -4181,8 +4181,8 @@
         <v>77</v>
       </c>
       <c r="C79" s="38">
-        <f>prevalence2018!C79/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C79/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -4193,8 +4193,8 @@
         <v>78</v>
       </c>
       <c r="C80" s="38">
-        <f>prevalence2018!C80/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C80/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -4205,8 +4205,8 @@
         <v>79</v>
       </c>
       <c r="C81" s="38">
-        <f>prevalence2018!C81/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C81/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -4217,8 +4217,8 @@
         <v>80</v>
       </c>
       <c r="C82" s="38">
-        <f>prevalence2018!C82/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C82/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -4229,8 +4229,8 @@
         <v>81</v>
       </c>
       <c r="C83" s="38">
-        <f>prevalence2018!C83/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C83/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -4241,8 +4241,8 @@
         <v>82</v>
       </c>
       <c r="C84" s="38">
-        <f>prevalence2018!C84/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C84/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -4253,8 +4253,8 @@
         <v>83</v>
       </c>
       <c r="C85" s="38">
-        <f>prevalence2018!C85/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C85/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -4265,8 +4265,8 @@
         <v>84</v>
       </c>
       <c r="C86" s="38">
-        <f>prevalence2018!C86/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C86/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -4277,8 +4277,8 @@
         <v>85</v>
       </c>
       <c r="C87" s="38">
-        <f>prevalence2018!C87/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C87/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -4289,8 +4289,8 @@
         <v>86</v>
       </c>
       <c r="C88" s="38">
-        <f>prevalence2018!C88/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C88/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -4301,8 +4301,8 @@
         <v>87</v>
       </c>
       <c r="C89" s="38">
-        <f>prevalence2018!C89/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C89/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -4313,8 +4313,8 @@
         <v>88</v>
       </c>
       <c r="C90" s="38">
-        <f>prevalence2018!C90/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C90/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -4325,8 +4325,8 @@
         <v>89</v>
       </c>
       <c r="C91" s="38">
-        <f>prevalence2018!C91/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C91/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -4337,8 +4337,8 @@
         <v>90</v>
       </c>
       <c r="C92" s="38">
-        <f>prevalence2018!C92/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C92/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -4349,8 +4349,8 @@
         <v>91</v>
       </c>
       <c r="C93" s="38">
-        <f>prevalence2018!C93/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C93/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -4361,8 +4361,8 @@
         <v>92</v>
       </c>
       <c r="C94" s="38">
-        <f>prevalence2018!C94/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C94/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -4373,8 +4373,8 @@
         <v>93</v>
       </c>
       <c r="C95" s="38">
-        <f>prevalence2018!C95/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C95/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -4385,8 +4385,8 @@
         <v>94</v>
       </c>
       <c r="C96" s="38">
-        <f>prevalence2018!C96/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C96/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -4397,8 +4397,8 @@
         <v>95</v>
       </c>
       <c r="C97" s="38">
-        <f>prevalence2018!C97/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C97/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -4409,8 +4409,8 @@
         <v>96</v>
       </c>
       <c r="C98" s="38">
-        <f>prevalence2018!C98/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C98/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -4421,8 +4421,8 @@
         <v>97</v>
       </c>
       <c r="C99" s="38">
-        <f>prevalence2018!C99/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C99/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -4433,8 +4433,8 @@
         <v>98</v>
       </c>
       <c r="C100" s="38">
-        <f>prevalence2018!C100/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C100/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -4445,8 +4445,8 @@
         <v>99</v>
       </c>
       <c r="C101" s="38">
-        <f>prevalence2018!C101/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C101/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -4457,8 +4457,8 @@
         <v>100</v>
       </c>
       <c r="C102" s="38">
-        <f>prevalence2018!C102/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C102/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -4469,8 +4469,8 @@
         <v>101</v>
       </c>
       <c r="C103" s="38">
-        <f>prevalence2018!C103/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C103/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -4481,8 +4481,8 @@
         <v>102</v>
       </c>
       <c r="C104" s="38">
-        <f>prevalence2018!C104/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C104/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -4493,8 +4493,8 @@
         <v>103</v>
       </c>
       <c r="C105" s="38">
-        <f>prevalence2018!C105/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C105/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -4505,8 +4505,8 @@
         <v>104</v>
       </c>
       <c r="C106" s="38">
-        <f>prevalence2018!C106/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C106/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -4517,8 +4517,8 @@
         <v>105</v>
       </c>
       <c r="C107" s="38">
-        <f>prevalence2018!C107/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C107/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -4529,8 +4529,8 @@
         <v>106</v>
       </c>
       <c r="C108" s="38">
-        <f>prevalence2018!C108/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C108/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -4541,8 +4541,8 @@
         <v>107</v>
       </c>
       <c r="C109" s="38">
-        <f>prevalence2018!C109/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C109/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -4553,8 +4553,8 @@
         <v>108</v>
       </c>
       <c r="C110" s="38">
-        <f>prevalence2018!C110/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C110/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -4565,8 +4565,8 @@
         <v>109</v>
       </c>
       <c r="C111" s="38">
-        <f>prevalence2018!C111/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C111/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -4577,8 +4577,8 @@
         <v>110</v>
       </c>
       <c r="C112" s="38">
-        <f>prevalence2018!C112/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C112/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -4589,8 +4589,8 @@
         <v>111</v>
       </c>
       <c r="C113" s="38">
-        <f>prevalence2018!C113/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C113/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -4601,8 +4601,8 @@
         <v>112</v>
       </c>
       <c r="C114" s="38">
-        <f>prevalence2018!C114/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C114/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -4613,8 +4613,8 @@
         <v>113</v>
       </c>
       <c r="C115" s="38">
-        <f>prevalence2018!C115/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C115/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -4625,8 +4625,8 @@
         <v>114</v>
       </c>
       <c r="C116" s="38">
-        <f>prevalence2018!C116/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C116/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -4637,8 +4637,8 @@
         <v>115</v>
       </c>
       <c r="C117" s="38">
-        <f>prevalence2018!C117/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C117/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -4649,8 +4649,8 @@
         <v>116</v>
       </c>
       <c r="C118" s="38">
-        <f>prevalence2018!C118/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C118/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -4661,8 +4661,8 @@
         <v>117</v>
       </c>
       <c r="C119" s="38">
-        <f>prevalence2018!C119/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C119/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -4673,8 +4673,8 @@
         <v>118</v>
       </c>
       <c r="C120" s="38">
-        <f>prevalence2018!C120/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C120/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -4685,8 +4685,8 @@
         <v>119</v>
       </c>
       <c r="C121" s="38">
-        <f>prevalence2018!C121/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C121/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -4697,8 +4697,8 @@
         <v>120</v>
       </c>
       <c r="C122" s="38">
-        <f>prevalence2018!C122/100</f>
-        <v>9.7000000000000003E-3</v>
+        <f>prevalence2018!C122/2</f>
+        <v>0.48499999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inicidence seems ok (WOOTWOOOT!). Outreach activated and scheduling referral.
To fix:
1. Log and plot
2. Read in 95% CI for plot
3. Trial outreach campaign
4. HSI event not running
5. Treatment with triage
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_HT.xlsx
+++ b/resources/ResourceFile_Method_HT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165FC138-1063-B64C-98F0-69418B7623A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60ED00A-622E-AA4B-A6D3-7C072AAA51BA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34140" yWindow="460" windowWidth="17060" windowHeight="26720" tabRatio="723" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3244,7 +3244,7 @@
   <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C27" sqref="C27:C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3554,8 +3554,8 @@
         <v>25</v>
       </c>
       <c r="C27" s="38">
-        <f>prevalence2018!C27/2</f>
-        <v>0.18</v>
+        <f>prevalence2018!C27/8</f>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3566,8 +3566,8 @@
         <v>26</v>
       </c>
       <c r="C28" s="38">
-        <f>prevalence2018!C28/2</f>
-        <v>0.18</v>
+        <f>prevalence2018!C28/8</f>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3578,8 +3578,8 @@
         <v>27</v>
       </c>
       <c r="C29" s="38">
-        <f>prevalence2018!C29/2</f>
-        <v>0.18</v>
+        <f>prevalence2018!C29/8</f>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3590,8 +3590,8 @@
         <v>28</v>
       </c>
       <c r="C30" s="38">
-        <f>prevalence2018!C30/2</f>
-        <v>0.18</v>
+        <f>prevalence2018!C30/8</f>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -3602,8 +3602,8 @@
         <v>29</v>
       </c>
       <c r="C31" s="38">
-        <f>prevalence2018!C31/2</f>
-        <v>0.18</v>
+        <f>prevalence2018!C31/8</f>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -3614,8 +3614,8 @@
         <v>30</v>
       </c>
       <c r="C32" s="38">
-        <f>prevalence2018!C32/2</f>
-        <v>0.18</v>
+        <f>prevalence2018!C32/8</f>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -3626,8 +3626,8 @@
         <v>31</v>
       </c>
       <c r="C33" s="38">
-        <f>prevalence2018!C33/2</f>
-        <v>0.18</v>
+        <f>prevalence2018!C33/8</f>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -3638,8 +3638,8 @@
         <v>32</v>
       </c>
       <c r="C34" s="38">
-        <f>prevalence2018!C34/2</f>
-        <v>0.18</v>
+        <f>prevalence2018!C34/8</f>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -3650,8 +3650,8 @@
         <v>33</v>
       </c>
       <c r="C35" s="38">
-        <f>prevalence2018!C35/2</f>
-        <v>0.18</v>
+        <f>prevalence2018!C35/8</f>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -3662,8 +3662,8 @@
         <v>34</v>
       </c>
       <c r="C36" s="38">
-        <f>prevalence2018!C36/2</f>
-        <v>0.18</v>
+        <f>prevalence2018!C36/8</f>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -3674,8 +3674,8 @@
         <v>35</v>
       </c>
       <c r="C37" s="38">
-        <f>prevalence2018!C37/2</f>
-        <v>0.21249999999999999</v>
+        <f>prevalence2018!C37/8</f>
+        <v>5.3124999999999999E-2</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -3686,8 +3686,8 @@
         <v>36</v>
       </c>
       <c r="C38" s="38">
-        <f>prevalence2018!C38/2</f>
-        <v>0.21249999999999999</v>
+        <f>prevalence2018!C38/8</f>
+        <v>5.3124999999999999E-2</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -3698,8 +3698,8 @@
         <v>37</v>
       </c>
       <c r="C39" s="38">
-        <f>prevalence2018!C39/2</f>
-        <v>0.21249999999999999</v>
+        <f>prevalence2018!C39/8</f>
+        <v>5.3124999999999999E-2</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -3710,8 +3710,8 @@
         <v>38</v>
       </c>
       <c r="C40" s="38">
-        <f>prevalence2018!C40/2</f>
-        <v>0.21249999999999999</v>
+        <f>prevalence2018!C40/8</f>
+        <v>5.3124999999999999E-2</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -3722,8 +3722,8 @@
         <v>39</v>
       </c>
       <c r="C41" s="38">
-        <f>prevalence2018!C41/2</f>
-        <v>0.21249999999999999</v>
+        <f>prevalence2018!C41/8</f>
+        <v>5.3124999999999999E-2</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -3734,8 +3734,8 @@
         <v>40</v>
       </c>
       <c r="C42" s="38">
-        <f>prevalence2018!C42/2</f>
-        <v>0.21249999999999999</v>
+        <f>prevalence2018!C42/8</f>
+        <v>5.3124999999999999E-2</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -3746,8 +3746,8 @@
         <v>41</v>
       </c>
       <c r="C43" s="38">
-        <f>prevalence2018!C43/2</f>
-        <v>0.21249999999999999</v>
+        <f>prevalence2018!C43/8</f>
+        <v>5.3124999999999999E-2</v>
       </c>
       <c r="I43" t="s">
         <v>60</v>
@@ -3761,8 +3761,8 @@
         <v>42</v>
       </c>
       <c r="C44" s="38">
-        <f>prevalence2018!C44/2</f>
-        <v>0.21249999999999999</v>
+        <f>prevalence2018!C44/8</f>
+        <v>5.3124999999999999E-2</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -3773,8 +3773,8 @@
         <v>43</v>
       </c>
       <c r="C45" s="38">
-        <f>prevalence2018!C45/2</f>
-        <v>0.21249999999999999</v>
+        <f>prevalence2018!C45/8</f>
+        <v>5.3124999999999999E-2</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -3785,8 +3785,8 @@
         <v>44</v>
       </c>
       <c r="C46" s="38">
-        <f>prevalence2018!C46/2</f>
-        <v>0.21249999999999999</v>
+        <f>prevalence2018!C46/8</f>
+        <v>5.3124999999999999E-2</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -3797,8 +3797,8 @@
         <v>45</v>
       </c>
       <c r="C47" s="38">
-        <f>prevalence2018!C47/2</f>
-        <v>0.25</v>
+        <f>prevalence2018!C47/8</f>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -3809,8 +3809,8 @@
         <v>46</v>
       </c>
       <c r="C48" s="38">
-        <f>prevalence2018!C48/2</f>
-        <v>0.25</v>
+        <f>prevalence2018!C48/8</f>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -3821,8 +3821,8 @@
         <v>47</v>
       </c>
       <c r="C49" s="38">
-        <f>prevalence2018!C49/2</f>
-        <v>0.25</v>
+        <f>prevalence2018!C49/8</f>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -3833,8 +3833,8 @@
         <v>48</v>
       </c>
       <c r="C50" s="38">
-        <f>prevalence2018!C50/2</f>
-        <v>0.25</v>
+        <f>prevalence2018!C50/8</f>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -3845,8 +3845,8 @@
         <v>49</v>
       </c>
       <c r="C51" s="38">
-        <f>prevalence2018!C51/2</f>
-        <v>0.25</v>
+        <f>prevalence2018!C51/8</f>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -3857,8 +3857,8 @@
         <v>50</v>
       </c>
       <c r="C52" s="38">
-        <f>prevalence2018!C52/2</f>
-        <v>0.25</v>
+        <f>prevalence2018!C52/8</f>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -3869,8 +3869,8 @@
         <v>51</v>
       </c>
       <c r="C53" s="38">
-        <f>prevalence2018!C53/2</f>
-        <v>0.25</v>
+        <f>prevalence2018!C53/8</f>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -3881,8 +3881,8 @@
         <v>52</v>
       </c>
       <c r="C54" s="38">
-        <f>prevalence2018!C54/2</f>
-        <v>0.25</v>
+        <f>prevalence2018!C54/8</f>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -3893,8 +3893,8 @@
         <v>53</v>
       </c>
       <c r="C55" s="38">
-        <f>prevalence2018!C55/2</f>
-        <v>0.25</v>
+        <f>prevalence2018!C55/8</f>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -3905,8 +3905,8 @@
         <v>54</v>
       </c>
       <c r="C56" s="38">
-        <f>prevalence2018!C56/2</f>
-        <v>0.25</v>
+        <f>prevalence2018!C56/8</f>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -3917,8 +3917,8 @@
         <v>55</v>
       </c>
       <c r="C57" s="38">
-        <f>prevalence2018!C57/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C57/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -3929,8 +3929,8 @@
         <v>56</v>
       </c>
       <c r="C58" s="38">
-        <f>prevalence2018!C58/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C58/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -3941,8 +3941,8 @@
         <v>57</v>
       </c>
       <c r="C59" s="38">
-        <f>prevalence2018!C59/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C59/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -3953,8 +3953,8 @@
         <v>58</v>
       </c>
       <c r="C60" s="38">
-        <f>prevalence2018!C60/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C60/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -3965,8 +3965,8 @@
         <v>59</v>
       </c>
       <c r="C61" s="38">
-        <f>prevalence2018!C61/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C61/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -3977,8 +3977,8 @@
         <v>60</v>
       </c>
       <c r="C62" s="38">
-        <f>prevalence2018!C62/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C62/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -3989,8 +3989,8 @@
         <v>61</v>
       </c>
       <c r="C63" s="38">
-        <f>prevalence2018!C63/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C63/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -4001,8 +4001,8 @@
         <v>62</v>
       </c>
       <c r="C64" s="38">
-        <f>prevalence2018!C64/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C64/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -4013,8 +4013,8 @@
         <v>63</v>
       </c>
       <c r="C65" s="38">
-        <f>prevalence2018!C65/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C65/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -4025,8 +4025,8 @@
         <v>64</v>
       </c>
       <c r="C66" s="38">
-        <f>prevalence2018!C66/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C66/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -4037,8 +4037,8 @@
         <v>65</v>
       </c>
       <c r="C67" s="38">
-        <f>prevalence2018!C67/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C67/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -4049,8 +4049,8 @@
         <v>66</v>
       </c>
       <c r="C68" s="38">
-        <f>prevalence2018!C68/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C68/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -4061,8 +4061,8 @@
         <v>67</v>
       </c>
       <c r="C69" s="38">
-        <f>prevalence2018!C69/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C69/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -4073,8 +4073,8 @@
         <v>68</v>
       </c>
       <c r="C70" s="38">
-        <f>prevalence2018!C70/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C70/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -4085,8 +4085,8 @@
         <v>69</v>
       </c>
       <c r="C71" s="38">
-        <f>prevalence2018!C71/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C71/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -4097,8 +4097,8 @@
         <v>70</v>
       </c>
       <c r="C72" s="38">
-        <f>prevalence2018!C72/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C72/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -4109,8 +4109,8 @@
         <v>71</v>
       </c>
       <c r="C73" s="38">
-        <f>prevalence2018!C73/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C73/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -4121,8 +4121,8 @@
         <v>72</v>
       </c>
       <c r="C74" s="38">
-        <f>prevalence2018!C74/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C74/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -4133,8 +4133,8 @@
         <v>73</v>
       </c>
       <c r="C75" s="38">
-        <f>prevalence2018!C75/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C75/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -4145,8 +4145,8 @@
         <v>74</v>
       </c>
       <c r="C76" s="38">
-        <f>prevalence2018!C76/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C76/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -4157,8 +4157,8 @@
         <v>75</v>
       </c>
       <c r="C77" s="38">
-        <f>prevalence2018!C77/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C77/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -4169,8 +4169,8 @@
         <v>76</v>
       </c>
       <c r="C78" s="38">
-        <f>prevalence2018!C78/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C78/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -4181,8 +4181,8 @@
         <v>77</v>
       </c>
       <c r="C79" s="38">
-        <f>prevalence2018!C79/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C79/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -4193,8 +4193,8 @@
         <v>78</v>
       </c>
       <c r="C80" s="38">
-        <f>prevalence2018!C80/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C80/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -4205,8 +4205,8 @@
         <v>79</v>
       </c>
       <c r="C81" s="38">
-        <f>prevalence2018!C81/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C81/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -4217,8 +4217,8 @@
         <v>80</v>
       </c>
       <c r="C82" s="38">
-        <f>prevalence2018!C82/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C82/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -4229,8 +4229,8 @@
         <v>81</v>
       </c>
       <c r="C83" s="38">
-        <f>prevalence2018!C83/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C83/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -4241,8 +4241,8 @@
         <v>82</v>
       </c>
       <c r="C84" s="38">
-        <f>prevalence2018!C84/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C84/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -4253,8 +4253,8 @@
         <v>83</v>
       </c>
       <c r="C85" s="38">
-        <f>prevalence2018!C85/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C85/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -4265,8 +4265,8 @@
         <v>84</v>
       </c>
       <c r="C86" s="38">
-        <f>prevalence2018!C86/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C86/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -4277,8 +4277,8 @@
         <v>85</v>
       </c>
       <c r="C87" s="38">
-        <f>prevalence2018!C87/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C87/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -4289,8 +4289,8 @@
         <v>86</v>
       </c>
       <c r="C88" s="38">
-        <f>prevalence2018!C88/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C88/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -4301,8 +4301,8 @@
         <v>87</v>
       </c>
       <c r="C89" s="38">
-        <f>prevalence2018!C89/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C89/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -4313,8 +4313,8 @@
         <v>88</v>
       </c>
       <c r="C90" s="38">
-        <f>prevalence2018!C90/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C90/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -4325,8 +4325,8 @@
         <v>89</v>
       </c>
       <c r="C91" s="38">
-        <f>prevalence2018!C91/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C91/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -4337,8 +4337,8 @@
         <v>90</v>
       </c>
       <c r="C92" s="38">
-        <f>prevalence2018!C92/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C92/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -4349,8 +4349,8 @@
         <v>91</v>
       </c>
       <c r="C93" s="38">
-        <f>prevalence2018!C93/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C93/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -4361,8 +4361,8 @@
         <v>92</v>
       </c>
       <c r="C94" s="38">
-        <f>prevalence2018!C94/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C94/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -4373,8 +4373,8 @@
         <v>93</v>
       </c>
       <c r="C95" s="38">
-        <f>prevalence2018!C95/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C95/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -4385,8 +4385,8 @@
         <v>94</v>
       </c>
       <c r="C96" s="38">
-        <f>prevalence2018!C96/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C96/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -4397,8 +4397,8 @@
         <v>95</v>
       </c>
       <c r="C97" s="38">
-        <f>prevalence2018!C97/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C97/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -4409,8 +4409,8 @@
         <v>96</v>
       </c>
       <c r="C98" s="38">
-        <f>prevalence2018!C98/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C98/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -4421,8 +4421,8 @@
         <v>97</v>
       </c>
       <c r="C99" s="38">
-        <f>prevalence2018!C99/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C99/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -4433,8 +4433,8 @@
         <v>98</v>
       </c>
       <c r="C100" s="38">
-        <f>prevalence2018!C100/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C100/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -4445,8 +4445,8 @@
         <v>99</v>
       </c>
       <c r="C101" s="38">
-        <f>prevalence2018!C101/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C101/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -4457,8 +4457,8 @@
         <v>100</v>
       </c>
       <c r="C102" s="38">
-        <f>prevalence2018!C102/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C102/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -4469,8 +4469,8 @@
         <v>101</v>
       </c>
       <c r="C103" s="38">
-        <f>prevalence2018!C103/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C103/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -4481,8 +4481,8 @@
         <v>102</v>
       </c>
       <c r="C104" s="38">
-        <f>prevalence2018!C104/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C104/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -4493,8 +4493,8 @@
         <v>103</v>
       </c>
       <c r="C105" s="38">
-        <f>prevalence2018!C105/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C105/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -4505,8 +4505,8 @@
         <v>104</v>
       </c>
       <c r="C106" s="38">
-        <f>prevalence2018!C106/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C106/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -4517,8 +4517,8 @@
         <v>105</v>
       </c>
       <c r="C107" s="38">
-        <f>prevalence2018!C107/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C107/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -4529,8 +4529,8 @@
         <v>106</v>
       </c>
       <c r="C108" s="38">
-        <f>prevalence2018!C108/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C108/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -4541,8 +4541,8 @@
         <v>107</v>
       </c>
       <c r="C109" s="38">
-        <f>prevalence2018!C109/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C109/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -4553,8 +4553,8 @@
         <v>108</v>
       </c>
       <c r="C110" s="38">
-        <f>prevalence2018!C110/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C110/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -4565,8 +4565,8 @@
         <v>109</v>
       </c>
       <c r="C111" s="38">
-        <f>prevalence2018!C111/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C111/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -4577,8 +4577,8 @@
         <v>110</v>
       </c>
       <c r="C112" s="38">
-        <f>prevalence2018!C112/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C112/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -4589,8 +4589,8 @@
         <v>111</v>
       </c>
       <c r="C113" s="38">
-        <f>prevalence2018!C113/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C113/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -4601,8 +4601,8 @@
         <v>112</v>
       </c>
       <c r="C114" s="38">
-        <f>prevalence2018!C114/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C114/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -4613,8 +4613,8 @@
         <v>113</v>
       </c>
       <c r="C115" s="38">
-        <f>prevalence2018!C115/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C115/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -4625,8 +4625,8 @@
         <v>114</v>
       </c>
       <c r="C116" s="38">
-        <f>prevalence2018!C116/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C116/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -4637,8 +4637,8 @@
         <v>115</v>
       </c>
       <c r="C117" s="38">
-        <f>prevalence2018!C117/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C117/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -4649,8 +4649,8 @@
         <v>116</v>
       </c>
       <c r="C118" s="38">
-        <f>prevalence2018!C118/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C118/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -4661,8 +4661,8 @@
         <v>117</v>
       </c>
       <c r="C119" s="38">
-        <f>prevalence2018!C119/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C119/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -4673,8 +4673,8 @@
         <v>118</v>
       </c>
       <c r="C120" s="38">
-        <f>prevalence2018!C120/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C120/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -4685,8 +4685,8 @@
         <v>119</v>
       </c>
       <c r="C121" s="38">
-        <f>prevalence2018!C121/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C121/8</f>
+        <v>0.12125</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -4697,8 +4697,8 @@
         <v>120</v>
       </c>
       <c r="C122" s="38">
-        <f>prevalence2018!C122/2</f>
-        <v>0.48499999999999999</v>
+        <f>prevalence2018!C122/8</f>
+        <v>0.12125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checks for random numbers at prev and inc
To Do:
1. Check prevalence
2. Check incidence
3. Add risk factors
4. Run test file
5. Log and plot
6. Read in 95% CI for plot
7. Trial outreach campaign
8. HSI event not running
9. Treatment with triage
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_HT.xlsx
+++ b/resources/ResourceFile_Method_HT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/PycharmProjects/TLOmodel/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/Dropbox/Projects - ongoing/Malawi Project/Thanzi la Onse/04 - Methods Repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60ED00A-622E-AA4B-A6D3-7C072AAA51BA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D192106-3F1F-D742-96A0-91576DF6592E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34140" yWindow="460" windowWidth="17060" windowHeight="26720" tabRatio="723" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6480" yWindow="460" windowWidth="17060" windowHeight="26720" tabRatio="723" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -1876,8 +1876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2185,7 +2185,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="38">
-        <v>0.36</v>
+        <v>0.21099999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2196,7 +2196,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="38">
-        <v>0.36</v>
+        <v>0.21099999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -2207,7 +2207,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="38">
-        <v>0.36</v>
+        <v>0.21099999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -2218,7 +2218,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="38">
-        <v>0.36</v>
+        <v>0.21099999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -2229,7 +2229,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="38">
-        <v>0.36</v>
+        <v>0.21099999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -2240,7 +2240,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="38">
-        <v>0.36</v>
+        <v>0.21099999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2251,7 +2251,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="38">
-        <v>0.36</v>
+        <v>0.21099999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2262,7 +2262,7 @@
         <v>32</v>
       </c>
       <c r="C34" s="38">
-        <v>0.36</v>
+        <v>0.21099999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2273,7 +2273,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="38">
-        <v>0.36</v>
+        <v>0.21099999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2284,7 +2284,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="38">
-        <v>0.36</v>
+        <v>0.21099999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2295,7 +2295,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="38">
-        <v>0.42499999999999999</v>
+        <v>0.314</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2306,7 +2306,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="38">
-        <v>0.42499999999999999</v>
+        <v>0.314</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2317,7 +2317,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="38">
-        <v>0.42499999999999999</v>
+        <v>0.314</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2328,7 +2328,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="38">
-        <v>0.42499999999999999</v>
+        <v>0.314</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2339,7 +2339,7 @@
         <v>39</v>
       </c>
       <c r="C41" s="38">
-        <v>0.42499999999999999</v>
+        <v>0.314</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2350,7 +2350,7 @@
         <v>40</v>
       </c>
       <c r="C42" s="38">
-        <v>0.42499999999999999</v>
+        <v>0.314</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2361,7 +2361,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="38">
-        <v>0.42499999999999999</v>
+        <v>0.314</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2372,7 +2372,7 @@
         <v>42</v>
       </c>
       <c r="C44" s="38">
-        <v>0.42499999999999999</v>
+        <v>0.314</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2383,7 +2383,7 @@
         <v>43</v>
       </c>
       <c r="C45" s="38">
-        <v>0.42499999999999999</v>
+        <v>0.314</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -2394,7 +2394,7 @@
         <v>44</v>
       </c>
       <c r="C46" s="38">
-        <v>0.42499999999999999</v>
+        <v>0.314</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -2405,7 +2405,7 @@
         <v>45</v>
       </c>
       <c r="C47" s="38">
-        <v>0.5</v>
+        <v>0.42899999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -2416,7 +2416,7 @@
         <v>46</v>
       </c>
       <c r="C48" s="38">
-        <v>0.5</v>
+        <v>0.42899999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -2427,7 +2427,7 @@
         <v>47</v>
       </c>
       <c r="C49" s="38">
-        <v>0.5</v>
+        <v>0.42899999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -2438,7 +2438,7 @@
         <v>48</v>
       </c>
       <c r="C50" s="38">
-        <v>0.5</v>
+        <v>0.42899999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -2449,7 +2449,7 @@
         <v>49</v>
       </c>
       <c r="C51" s="38">
-        <v>0.5</v>
+        <v>0.42899999999999999</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -2460,7 +2460,7 @@
         <v>50</v>
       </c>
       <c r="C52" s="38">
-        <v>0.5</v>
+        <v>0.42899999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -2471,7 +2471,7 @@
         <v>51</v>
       </c>
       <c r="C53" s="38">
-        <v>0.5</v>
+        <v>0.42899999999999999</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -2482,7 +2482,7 @@
         <v>52</v>
       </c>
       <c r="C54" s="38">
-        <v>0.5</v>
+        <v>0.42899999999999999</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -2493,7 +2493,7 @@
         <v>53</v>
       </c>
       <c r="C55" s="38">
-        <v>0.5</v>
+        <v>0.42899999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -2504,7 +2504,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="38">
-        <v>0.5</v>
+        <v>0.42899999999999999</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2515,7 +2515,7 @@
         <v>55</v>
       </c>
       <c r="C57" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2526,7 +2526,7 @@
         <v>56</v>
       </c>
       <c r="C58" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -2537,7 +2537,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -2548,7 +2548,7 @@
         <v>58</v>
       </c>
       <c r="C60" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -2559,7 +2559,7 @@
         <v>59</v>
       </c>
       <c r="C61" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -2570,7 +2570,7 @@
         <v>60</v>
       </c>
       <c r="C62" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -2581,7 +2581,7 @@
         <v>61</v>
       </c>
       <c r="C63" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -2592,7 +2592,7 @@
         <v>62</v>
       </c>
       <c r="C64" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -2603,7 +2603,7 @@
         <v>63</v>
       </c>
       <c r="C65" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -2614,7 +2614,7 @@
         <v>64</v>
       </c>
       <c r="C66" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -2625,7 +2625,7 @@
         <v>65</v>
       </c>
       <c r="C67" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -2636,7 +2636,7 @@
         <v>66</v>
       </c>
       <c r="C68" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -2647,7 +2647,7 @@
         <v>67</v>
       </c>
       <c r="C69" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -2658,7 +2658,7 @@
         <v>68</v>
       </c>
       <c r="C70" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -2669,7 +2669,7 @@
         <v>69</v>
       </c>
       <c r="C71" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -2680,7 +2680,7 @@
         <v>70</v>
       </c>
       <c r="C72" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -2691,7 +2691,7 @@
         <v>71</v>
       </c>
       <c r="C73" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -2702,7 +2702,7 @@
         <v>72</v>
       </c>
       <c r="C74" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -2713,7 +2713,7 @@
         <v>73</v>
       </c>
       <c r="C75" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -2724,7 +2724,7 @@
         <v>74</v>
       </c>
       <c r="C76" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -2735,7 +2735,7 @@
         <v>75</v>
       </c>
       <c r="C77" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -2746,7 +2746,7 @@
         <v>76</v>
       </c>
       <c r="C78" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -2757,7 +2757,7 @@
         <v>77</v>
       </c>
       <c r="C79" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -2768,7 +2768,7 @@
         <v>78</v>
       </c>
       <c r="C80" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -2779,7 +2779,7 @@
         <v>79</v>
       </c>
       <c r="C81" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -2790,7 +2790,7 @@
         <v>80</v>
       </c>
       <c r="C82" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -2801,7 +2801,7 @@
         <v>81</v>
       </c>
       <c r="C83" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -2812,7 +2812,7 @@
         <v>82</v>
       </c>
       <c r="C84" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -2823,7 +2823,7 @@
         <v>83</v>
       </c>
       <c r="C85" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -2834,7 +2834,7 @@
         <v>84</v>
       </c>
       <c r="C86" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -2845,7 +2845,7 @@
         <v>85</v>
       </c>
       <c r="C87" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -2856,7 +2856,7 @@
         <v>86</v>
       </c>
       <c r="C88" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -2867,7 +2867,7 @@
         <v>87</v>
       </c>
       <c r="C89" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -2878,7 +2878,7 @@
         <v>88</v>
       </c>
       <c r="C90" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -2889,7 +2889,7 @@
         <v>89</v>
       </c>
       <c r="C91" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -2900,7 +2900,7 @@
         <v>90</v>
       </c>
       <c r="C92" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -2911,7 +2911,7 @@
         <v>91</v>
       </c>
       <c r="C93" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -2922,7 +2922,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -2933,7 +2933,7 @@
         <v>93</v>
       </c>
       <c r="C95" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -2944,7 +2944,7 @@
         <v>94</v>
       </c>
       <c r="C96" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -2955,7 +2955,7 @@
         <v>95</v>
       </c>
       <c r="C97" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -2966,7 +2966,7 @@
         <v>96</v>
       </c>
       <c r="C98" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -2977,7 +2977,7 @@
         <v>97</v>
       </c>
       <c r="C99" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -2988,7 +2988,7 @@
         <v>98</v>
       </c>
       <c r="C100" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -2999,7 +2999,7 @@
         <v>99</v>
       </c>
       <c r="C101" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -3010,7 +3010,7 @@
         <v>100</v>
       </c>
       <c r="C102" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -3021,7 +3021,7 @@
         <v>101</v>
       </c>
       <c r="C103" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -3032,7 +3032,7 @@
         <v>102</v>
       </c>
       <c r="C104" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -3043,7 +3043,7 @@
         <v>103</v>
       </c>
       <c r="C105" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -3054,7 +3054,7 @@
         <v>104</v>
       </c>
       <c r="C106" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -3065,7 +3065,7 @@
         <v>105</v>
       </c>
       <c r="C107" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -3076,7 +3076,7 @@
         <v>106</v>
       </c>
       <c r="C108" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -3087,7 +3087,7 @@
         <v>107</v>
       </c>
       <c r="C109" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -3098,7 +3098,7 @@
         <v>108</v>
       </c>
       <c r="C110" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -3109,7 +3109,7 @@
         <v>109</v>
       </c>
       <c r="C111" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -3120,7 +3120,7 @@
         <v>110</v>
       </c>
       <c r="C112" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -3131,7 +3131,7 @@
         <v>111</v>
       </c>
       <c r="C113" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -3142,7 +3142,7 @@
         <v>112</v>
       </c>
       <c r="C114" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -3153,7 +3153,7 @@
         <v>113</v>
       </c>
       <c r="C115" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -3164,7 +3164,7 @@
         <v>114</v>
       </c>
       <c r="C116" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -3175,7 +3175,7 @@
         <v>115</v>
       </c>
       <c r="C117" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -3186,7 +3186,7 @@
         <v>116</v>
       </c>
       <c r="C118" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -3197,7 +3197,7 @@
         <v>117</v>
       </c>
       <c r="C119" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -3208,7 +3208,7 @@
         <v>118</v>
       </c>
       <c r="C120" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -3219,7 +3219,7 @@
         <v>119</v>
       </c>
       <c r="C121" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -3230,7 +3230,7 @@
         <v>120</v>
       </c>
       <c r="C122" s="38">
-        <v>0.97</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -3243,8 +3243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:C122"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3554,8 +3554,8 @@
         <v>25</v>
       </c>
       <c r="C27" s="38">
-        <f>prevalence2018!C27/8</f>
-        <v>4.4999999999999998E-2</v>
+        <f>prevalence2018!C27/2</f>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3566,8 +3566,8 @@
         <v>26</v>
       </c>
       <c r="C28" s="38">
-        <f>prevalence2018!C28/8</f>
-        <v>4.4999999999999998E-2</v>
+        <f>prevalence2018!C28/2</f>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3578,8 +3578,8 @@
         <v>27</v>
       </c>
       <c r="C29" s="38">
-        <f>prevalence2018!C29/8</f>
-        <v>4.4999999999999998E-2</v>
+        <f>prevalence2018!C29/2</f>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3590,8 +3590,8 @@
         <v>28</v>
       </c>
       <c r="C30" s="38">
-        <f>prevalence2018!C30/8</f>
-        <v>4.4999999999999998E-2</v>
+        <f>prevalence2018!C30/2</f>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -3602,8 +3602,8 @@
         <v>29</v>
       </c>
       <c r="C31" s="38">
-        <f>prevalence2018!C31/8</f>
-        <v>4.4999999999999998E-2</v>
+        <f>prevalence2018!C31/2</f>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -3614,8 +3614,8 @@
         <v>30</v>
       </c>
       <c r="C32" s="38">
-        <f>prevalence2018!C32/8</f>
-        <v>4.4999999999999998E-2</v>
+        <f>prevalence2018!C32/2</f>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -3626,8 +3626,8 @@
         <v>31</v>
       </c>
       <c r="C33" s="38">
-        <f>prevalence2018!C33/8</f>
-        <v>4.4999999999999998E-2</v>
+        <f>prevalence2018!C33/2</f>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -3638,8 +3638,8 @@
         <v>32</v>
       </c>
       <c r="C34" s="38">
-        <f>prevalence2018!C34/8</f>
-        <v>4.4999999999999998E-2</v>
+        <f>prevalence2018!C34/2</f>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -3650,8 +3650,8 @@
         <v>33</v>
       </c>
       <c r="C35" s="38">
-        <f>prevalence2018!C35/8</f>
-        <v>4.4999999999999998E-2</v>
+        <f>prevalence2018!C35/2</f>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -3662,8 +3662,8 @@
         <v>34</v>
       </c>
       <c r="C36" s="38">
-        <f>prevalence2018!C36/8</f>
-        <v>4.4999999999999998E-2</v>
+        <f>prevalence2018!C36/2</f>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -3674,8 +3674,8 @@
         <v>35</v>
       </c>
       <c r="C37" s="38">
-        <f>prevalence2018!C37/8</f>
-        <v>5.3124999999999999E-2</v>
+        <f>prevalence2018!C37/2</f>
+        <v>0.157</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -3686,8 +3686,8 @@
         <v>36</v>
       </c>
       <c r="C38" s="38">
-        <f>prevalence2018!C38/8</f>
-        <v>5.3124999999999999E-2</v>
+        <f>prevalence2018!C38/2</f>
+        <v>0.157</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -3698,8 +3698,8 @@
         <v>37</v>
       </c>
       <c r="C39" s="38">
-        <f>prevalence2018!C39/8</f>
-        <v>5.3124999999999999E-2</v>
+        <f>prevalence2018!C39/2</f>
+        <v>0.157</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -3710,8 +3710,8 @@
         <v>38</v>
       </c>
       <c r="C40" s="38">
-        <f>prevalence2018!C40/8</f>
-        <v>5.3124999999999999E-2</v>
+        <f>prevalence2018!C40/2</f>
+        <v>0.157</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -3722,8 +3722,8 @@
         <v>39</v>
       </c>
       <c r="C41" s="38">
-        <f>prevalence2018!C41/8</f>
-        <v>5.3124999999999999E-2</v>
+        <f>prevalence2018!C41/2</f>
+        <v>0.157</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -3734,8 +3734,8 @@
         <v>40</v>
       </c>
       <c r="C42" s="38">
-        <f>prevalence2018!C42/8</f>
-        <v>5.3124999999999999E-2</v>
+        <f>prevalence2018!C42/2</f>
+        <v>0.157</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -3746,8 +3746,8 @@
         <v>41</v>
       </c>
       <c r="C43" s="38">
-        <f>prevalence2018!C43/8</f>
-        <v>5.3124999999999999E-2</v>
+        <f>prevalence2018!C43/2</f>
+        <v>0.157</v>
       </c>
       <c r="I43" t="s">
         <v>60</v>
@@ -3761,8 +3761,8 @@
         <v>42</v>
       </c>
       <c r="C44" s="38">
-        <f>prevalence2018!C44/8</f>
-        <v>5.3124999999999999E-2</v>
+        <f>prevalence2018!C44/2</f>
+        <v>0.157</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -3773,8 +3773,8 @@
         <v>43</v>
       </c>
       <c r="C45" s="38">
-        <f>prevalence2018!C45/8</f>
-        <v>5.3124999999999999E-2</v>
+        <f>prevalence2018!C45/2</f>
+        <v>0.157</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -3785,8 +3785,8 @@
         <v>44</v>
       </c>
       <c r="C46" s="38">
-        <f>prevalence2018!C46/8</f>
-        <v>5.3124999999999999E-2</v>
+        <f>prevalence2018!C46/2</f>
+        <v>0.157</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -3797,8 +3797,8 @@
         <v>45</v>
       </c>
       <c r="C47" s="38">
-        <f>prevalence2018!C47/8</f>
-        <v>6.25E-2</v>
+        <f>prevalence2018!C47/2</f>
+        <v>0.2145</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -3809,8 +3809,8 @@
         <v>46</v>
       </c>
       <c r="C48" s="38">
-        <f>prevalence2018!C48/8</f>
-        <v>6.25E-2</v>
+        <f>prevalence2018!C48/2</f>
+        <v>0.2145</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -3821,8 +3821,8 @@
         <v>47</v>
       </c>
       <c r="C49" s="38">
-        <f>prevalence2018!C49/8</f>
-        <v>6.25E-2</v>
+        <f>prevalence2018!C49/2</f>
+        <v>0.2145</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -3833,8 +3833,8 @@
         <v>48</v>
       </c>
       <c r="C50" s="38">
-        <f>prevalence2018!C50/8</f>
-        <v>6.25E-2</v>
+        <f>prevalence2018!C50/2</f>
+        <v>0.2145</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -3845,8 +3845,8 @@
         <v>49</v>
       </c>
       <c r="C51" s="38">
-        <f>prevalence2018!C51/8</f>
-        <v>6.25E-2</v>
+        <f>prevalence2018!C51/2</f>
+        <v>0.2145</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -3857,8 +3857,8 @@
         <v>50</v>
       </c>
       <c r="C52" s="38">
-        <f>prevalence2018!C52/8</f>
-        <v>6.25E-2</v>
+        <f>prevalence2018!C52/2</f>
+        <v>0.2145</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -3869,8 +3869,8 @@
         <v>51</v>
       </c>
       <c r="C53" s="38">
-        <f>prevalence2018!C53/8</f>
-        <v>6.25E-2</v>
+        <f>prevalence2018!C53/2</f>
+        <v>0.2145</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -3881,8 +3881,8 @@
         <v>52</v>
       </c>
       <c r="C54" s="38">
-        <f>prevalence2018!C54/8</f>
-        <v>6.25E-2</v>
+        <f>prevalence2018!C54/2</f>
+        <v>0.2145</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -3893,8 +3893,8 @@
         <v>53</v>
       </c>
       <c r="C55" s="38">
-        <f>prevalence2018!C55/8</f>
-        <v>6.25E-2</v>
+        <f>prevalence2018!C55/2</f>
+        <v>0.2145</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -3905,8 +3905,8 @@
         <v>54</v>
       </c>
       <c r="C56" s="38">
-        <f>prevalence2018!C56/8</f>
-        <v>6.25E-2</v>
+        <f>prevalence2018!C56/2</f>
+        <v>0.2145</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -3917,8 +3917,8 @@
         <v>55</v>
       </c>
       <c r="C57" s="38">
-        <f>prevalence2018!C57/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C57/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -3929,8 +3929,8 @@
         <v>56</v>
       </c>
       <c r="C58" s="38">
-        <f>prevalence2018!C58/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C58/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -3941,8 +3941,8 @@
         <v>57</v>
       </c>
       <c r="C59" s="38">
-        <f>prevalence2018!C59/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C59/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -3953,8 +3953,8 @@
         <v>58</v>
       </c>
       <c r="C60" s="38">
-        <f>prevalence2018!C60/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C60/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -3965,8 +3965,8 @@
         <v>59</v>
       </c>
       <c r="C61" s="38">
-        <f>prevalence2018!C61/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C61/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -3977,8 +3977,8 @@
         <v>60</v>
       </c>
       <c r="C62" s="38">
-        <f>prevalence2018!C62/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C62/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -3989,8 +3989,8 @@
         <v>61</v>
       </c>
       <c r="C63" s="38">
-        <f>prevalence2018!C63/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C63/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -4001,8 +4001,8 @@
         <v>62</v>
       </c>
       <c r="C64" s="38">
-        <f>prevalence2018!C64/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C64/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -4013,8 +4013,8 @@
         <v>63</v>
       </c>
       <c r="C65" s="38">
-        <f>prevalence2018!C65/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C65/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -4025,8 +4025,8 @@
         <v>64</v>
       </c>
       <c r="C66" s="38">
-        <f>prevalence2018!C66/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C66/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -4037,8 +4037,8 @@
         <v>65</v>
       </c>
       <c r="C67" s="38">
-        <f>prevalence2018!C67/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C67/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -4049,8 +4049,8 @@
         <v>66</v>
       </c>
       <c r="C68" s="38">
-        <f>prevalence2018!C68/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C68/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -4061,8 +4061,8 @@
         <v>67</v>
       </c>
       <c r="C69" s="38">
-        <f>prevalence2018!C69/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C69/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -4073,8 +4073,8 @@
         <v>68</v>
       </c>
       <c r="C70" s="38">
-        <f>prevalence2018!C70/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C70/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -4085,8 +4085,8 @@
         <v>69</v>
       </c>
       <c r="C71" s="38">
-        <f>prevalence2018!C71/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C71/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -4097,8 +4097,8 @@
         <v>70</v>
       </c>
       <c r="C72" s="38">
-        <f>prevalence2018!C72/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C72/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -4109,8 +4109,8 @@
         <v>71</v>
       </c>
       <c r="C73" s="38">
-        <f>prevalence2018!C73/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C73/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -4121,8 +4121,8 @@
         <v>72</v>
       </c>
       <c r="C74" s="38">
-        <f>prevalence2018!C74/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C74/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -4133,8 +4133,8 @@
         <v>73</v>
       </c>
       <c r="C75" s="38">
-        <f>prevalence2018!C75/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C75/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -4145,8 +4145,8 @@
         <v>74</v>
       </c>
       <c r="C76" s="38">
-        <f>prevalence2018!C76/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C76/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -4157,8 +4157,8 @@
         <v>75</v>
       </c>
       <c r="C77" s="38">
-        <f>prevalence2018!C77/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C77/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -4169,8 +4169,8 @@
         <v>76</v>
       </c>
       <c r="C78" s="38">
-        <f>prevalence2018!C78/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C78/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -4181,8 +4181,8 @@
         <v>77</v>
       </c>
       <c r="C79" s="38">
-        <f>prevalence2018!C79/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C79/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -4193,8 +4193,8 @@
         <v>78</v>
       </c>
       <c r="C80" s="38">
-        <f>prevalence2018!C80/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C80/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -4205,8 +4205,8 @@
         <v>79</v>
       </c>
       <c r="C81" s="38">
-        <f>prevalence2018!C81/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C81/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -4217,8 +4217,8 @@
         <v>80</v>
       </c>
       <c r="C82" s="38">
-        <f>prevalence2018!C82/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C82/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -4229,8 +4229,8 @@
         <v>81</v>
       </c>
       <c r="C83" s="38">
-        <f>prevalence2018!C83/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C83/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -4241,8 +4241,8 @@
         <v>82</v>
       </c>
       <c r="C84" s="38">
-        <f>prevalence2018!C84/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C84/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -4253,8 +4253,8 @@
         <v>83</v>
       </c>
       <c r="C85" s="38">
-        <f>prevalence2018!C85/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C85/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -4265,8 +4265,8 @@
         <v>84</v>
       </c>
       <c r="C86" s="38">
-        <f>prevalence2018!C86/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C86/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -4277,8 +4277,8 @@
         <v>85</v>
       </c>
       <c r="C87" s="38">
-        <f>prevalence2018!C87/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C87/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -4289,8 +4289,8 @@
         <v>86</v>
       </c>
       <c r="C88" s="38">
-        <f>prevalence2018!C88/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C88/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -4301,8 +4301,8 @@
         <v>87</v>
       </c>
       <c r="C89" s="38">
-        <f>prevalence2018!C89/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C89/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -4313,8 +4313,8 @@
         <v>88</v>
       </c>
       <c r="C90" s="38">
-        <f>prevalence2018!C90/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C90/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -4325,8 +4325,8 @@
         <v>89</v>
       </c>
       <c r="C91" s="38">
-        <f>prevalence2018!C91/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C91/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -4337,8 +4337,8 @@
         <v>90</v>
       </c>
       <c r="C92" s="38">
-        <f>prevalence2018!C92/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C92/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -4349,8 +4349,8 @@
         <v>91</v>
       </c>
       <c r="C93" s="38">
-        <f>prevalence2018!C93/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C93/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -4361,8 +4361,8 @@
         <v>92</v>
       </c>
       <c r="C94" s="38">
-        <f>prevalence2018!C94/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C94/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -4373,8 +4373,8 @@
         <v>93</v>
       </c>
       <c r="C95" s="38">
-        <f>prevalence2018!C95/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C95/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -4385,8 +4385,8 @@
         <v>94</v>
       </c>
       <c r="C96" s="38">
-        <f>prevalence2018!C96/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C96/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -4397,8 +4397,8 @@
         <v>95</v>
       </c>
       <c r="C97" s="38">
-        <f>prevalence2018!C97/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C97/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -4409,8 +4409,8 @@
         <v>96</v>
       </c>
       <c r="C98" s="38">
-        <f>prevalence2018!C98/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C98/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -4421,8 +4421,8 @@
         <v>97</v>
       </c>
       <c r="C99" s="38">
-        <f>prevalence2018!C99/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C99/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -4433,8 +4433,8 @@
         <v>98</v>
       </c>
       <c r="C100" s="38">
-        <f>prevalence2018!C100/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C100/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -4445,8 +4445,8 @@
         <v>99</v>
       </c>
       <c r="C101" s="38">
-        <f>prevalence2018!C101/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C101/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -4457,8 +4457,8 @@
         <v>100</v>
       </c>
       <c r="C102" s="38">
-        <f>prevalence2018!C102/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C102/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -4469,8 +4469,8 @@
         <v>101</v>
       </c>
       <c r="C103" s="38">
-        <f>prevalence2018!C103/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C103/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -4481,8 +4481,8 @@
         <v>102</v>
       </c>
       <c r="C104" s="38">
-        <f>prevalence2018!C104/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C104/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -4493,8 +4493,8 @@
         <v>103</v>
       </c>
       <c r="C105" s="38">
-        <f>prevalence2018!C105/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C105/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -4505,8 +4505,8 @@
         <v>104</v>
       </c>
       <c r="C106" s="38">
-        <f>prevalence2018!C106/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C106/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -4517,8 +4517,8 @@
         <v>105</v>
       </c>
       <c r="C107" s="38">
-        <f>prevalence2018!C107/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C107/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -4529,8 +4529,8 @@
         <v>106</v>
       </c>
       <c r="C108" s="38">
-        <f>prevalence2018!C108/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C108/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -4541,8 +4541,8 @@
         <v>107</v>
       </c>
       <c r="C109" s="38">
-        <f>prevalence2018!C109/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C109/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -4553,8 +4553,8 @@
         <v>108</v>
       </c>
       <c r="C110" s="38">
-        <f>prevalence2018!C110/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C110/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -4565,8 +4565,8 @@
         <v>109</v>
       </c>
       <c r="C111" s="38">
-        <f>prevalence2018!C111/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C111/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -4577,8 +4577,8 @@
         <v>110</v>
       </c>
       <c r="C112" s="38">
-        <f>prevalence2018!C112/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C112/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -4589,8 +4589,8 @@
         <v>111</v>
       </c>
       <c r="C113" s="38">
-        <f>prevalence2018!C113/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C113/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -4601,8 +4601,8 @@
         <v>112</v>
       </c>
       <c r="C114" s="38">
-        <f>prevalence2018!C114/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C114/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -4613,8 +4613,8 @@
         <v>113</v>
       </c>
       <c r="C115" s="38">
-        <f>prevalence2018!C115/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C115/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -4625,8 +4625,8 @@
         <v>114</v>
       </c>
       <c r="C116" s="38">
-        <f>prevalence2018!C116/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C116/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -4637,8 +4637,8 @@
         <v>115</v>
       </c>
       <c r="C117" s="38">
-        <f>prevalence2018!C117/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C117/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -4649,8 +4649,8 @@
         <v>116</v>
       </c>
       <c r="C118" s="38">
-        <f>prevalence2018!C118/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C118/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -4661,8 +4661,8 @@
         <v>117</v>
       </c>
       <c r="C119" s="38">
-        <f>prevalence2018!C119/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C119/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -4673,8 +4673,8 @@
         <v>118</v>
       </c>
       <c r="C120" s="38">
-        <f>prevalence2018!C120/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C120/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -4685,8 +4685,8 @@
         <v>119</v>
       </c>
       <c r="C121" s="38">
-        <f>prevalence2018!C121/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C121/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -4697,8 +4697,8 @@
         <v>120</v>
       </c>
       <c r="C122" s="38">
-        <f>prevalence2018!C122/8</f>
-        <v>0.12125</v>
+        <f>prevalence2018!C122/2</f>
+        <v>0.29649999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T2DM working and in line
To do
1. Finalise HTN prev and Diab with HR
2. Log and Plot
3. clean up (remove FH)
4. HSI event flesh out HTN
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_HT.xlsx
+++ b/resources/ResourceFile_Method_HT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/Dropbox/Projects - ongoing/Malawi Project/Thanzi la Onse/04 - Methods Repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D192106-3F1F-D742-96A0-91576DF6592E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CC8026-A282-A54B-9975-77FD01E66026}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="460" windowWidth="17060" windowHeight="26720" tabRatio="723" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="15860" tabRatio="723" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1876,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27:E31"/>
+    <sheetView topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57:C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2185,7 +2183,8 @@
         <v>25</v>
       </c>
       <c r="C27" s="38">
-        <v>0.21099999999999999</v>
+        <f>0.211*0.82</f>
+        <v>0.17301999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2196,7 +2195,8 @@
         <v>26</v>
       </c>
       <c r="C28" s="38">
-        <v>0.21099999999999999</v>
+        <f t="shared" ref="C28:C36" si="0">0.211*0.82</f>
+        <v>0.17301999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -2207,7 +2207,8 @@
         <v>27</v>
       </c>
       <c r="C29" s="38">
-        <v>0.21099999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.17301999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -2218,7 +2219,8 @@
         <v>28</v>
       </c>
       <c r="C30" s="38">
-        <v>0.21099999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.17301999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -2229,7 +2231,8 @@
         <v>29</v>
       </c>
       <c r="C31" s="38">
-        <v>0.21099999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.17301999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -2240,7 +2243,8 @@
         <v>30</v>
       </c>
       <c r="C32" s="38">
-        <v>0.21099999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.17301999999999998</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2251,7 +2255,8 @@
         <v>31</v>
       </c>
       <c r="C33" s="38">
-        <v>0.21099999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.17301999999999998</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2262,7 +2267,8 @@
         <v>32</v>
       </c>
       <c r="C34" s="38">
-        <v>0.21099999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.17301999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2273,7 +2279,8 @@
         <v>33</v>
       </c>
       <c r="C35" s="38">
-        <v>0.21099999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.17301999999999998</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2284,7 +2291,8 @@
         <v>34</v>
       </c>
       <c r="C36" s="38">
-        <v>0.21099999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.17301999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2295,7 +2303,8 @@
         <v>35</v>
       </c>
       <c r="C37" s="38">
-        <v>0.314</v>
+        <f>0.314*0.81</f>
+        <v>0.25434000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2306,7 +2315,8 @@
         <v>36</v>
       </c>
       <c r="C38" s="38">
-        <v>0.314</v>
+        <f t="shared" ref="C38:C46" si="1">0.314*0.81</f>
+        <v>0.25434000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2317,7 +2327,8 @@
         <v>37</v>
       </c>
       <c r="C39" s="38">
-        <v>0.314</v>
+        <f t="shared" si="1"/>
+        <v>0.25434000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2328,7 +2339,8 @@
         <v>38</v>
       </c>
       <c r="C40" s="38">
-        <v>0.314</v>
+        <f t="shared" si="1"/>
+        <v>0.25434000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2339,7 +2351,8 @@
         <v>39</v>
       </c>
       <c r="C41" s="38">
-        <v>0.314</v>
+        <f t="shared" si="1"/>
+        <v>0.25434000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2350,7 +2363,8 @@
         <v>40</v>
       </c>
       <c r="C42" s="38">
-        <v>0.314</v>
+        <f t="shared" si="1"/>
+        <v>0.25434000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2361,7 +2375,8 @@
         <v>41</v>
       </c>
       <c r="C43" s="38">
-        <v>0.314</v>
+        <f t="shared" si="1"/>
+        <v>0.25434000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2372,7 +2387,8 @@
         <v>42</v>
       </c>
       <c r="C44" s="38">
-        <v>0.314</v>
+        <f t="shared" si="1"/>
+        <v>0.25434000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2383,7 +2399,8 @@
         <v>43</v>
       </c>
       <c r="C45" s="38">
-        <v>0.314</v>
+        <f t="shared" si="1"/>
+        <v>0.25434000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -2394,7 +2411,8 @@
         <v>44</v>
       </c>
       <c r="C46" s="38">
-        <v>0.314</v>
+        <f t="shared" si="1"/>
+        <v>0.25434000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -2405,7 +2423,8 @@
         <v>45</v>
       </c>
       <c r="C47" s="38">
-        <v>0.42899999999999999</v>
+        <f>0.429*0.82</f>
+        <v>0.35177999999999998</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -2416,7 +2435,8 @@
         <v>46</v>
       </c>
       <c r="C48" s="38">
-        <v>0.42899999999999999</v>
+        <f t="shared" ref="C48:C56" si="2">0.429*0.82</f>
+        <v>0.35177999999999998</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -2427,7 +2447,8 @@
         <v>47</v>
       </c>
       <c r="C49" s="38">
-        <v>0.42899999999999999</v>
+        <f t="shared" si="2"/>
+        <v>0.35177999999999998</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -2438,7 +2459,8 @@
         <v>48</v>
       </c>
       <c r="C50" s="38">
-        <v>0.42899999999999999</v>
+        <f t="shared" si="2"/>
+        <v>0.35177999999999998</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -2449,7 +2471,8 @@
         <v>49</v>
       </c>
       <c r="C51" s="38">
-        <v>0.42899999999999999</v>
+        <f t="shared" si="2"/>
+        <v>0.35177999999999998</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -2460,7 +2483,8 @@
         <v>50</v>
       </c>
       <c r="C52" s="38">
-        <v>0.42899999999999999</v>
+        <f t="shared" si="2"/>
+        <v>0.35177999999999998</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -2471,7 +2495,8 @@
         <v>51</v>
       </c>
       <c r="C53" s="38">
-        <v>0.42899999999999999</v>
+        <f t="shared" si="2"/>
+        <v>0.35177999999999998</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -2482,7 +2507,8 @@
         <v>52</v>
       </c>
       <c r="C54" s="38">
-        <v>0.42899999999999999</v>
+        <f t="shared" si="2"/>
+        <v>0.35177999999999998</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -2493,7 +2519,8 @@
         <v>53</v>
       </c>
       <c r="C55" s="38">
-        <v>0.42899999999999999</v>
+        <f t="shared" si="2"/>
+        <v>0.35177999999999998</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -2504,7 +2531,8 @@
         <v>54</v>
       </c>
       <c r="C56" s="38">
-        <v>0.42899999999999999</v>
+        <f t="shared" si="2"/>
+        <v>0.35177999999999998</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2515,7 +2543,8 @@
         <v>55</v>
       </c>
       <c r="C57" s="38">
-        <v>0.59299999999999997</v>
+        <f>0.593*0.82</f>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2526,7 +2555,8 @@
         <v>56</v>
       </c>
       <c r="C58" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" ref="C58:C121" si="3">0.593*0.82</f>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -2537,7 +2567,8 @@
         <v>57</v>
       </c>
       <c r="C59" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -2548,7 +2579,8 @@
         <v>58</v>
       </c>
       <c r="C60" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -2559,7 +2591,8 @@
         <v>59</v>
       </c>
       <c r="C61" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -2570,7 +2603,8 @@
         <v>60</v>
       </c>
       <c r="C62" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -2581,7 +2615,8 @@
         <v>61</v>
       </c>
       <c r="C63" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -2592,7 +2627,8 @@
         <v>62</v>
       </c>
       <c r="C64" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -2603,7 +2639,8 @@
         <v>63</v>
       </c>
       <c r="C65" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -2614,7 +2651,8 @@
         <v>64</v>
       </c>
       <c r="C66" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -2625,7 +2663,8 @@
         <v>65</v>
       </c>
       <c r="C67" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -2636,7 +2675,8 @@
         <v>66</v>
       </c>
       <c r="C68" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -2647,7 +2687,8 @@
         <v>67</v>
       </c>
       <c r="C69" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -2658,7 +2699,8 @@
         <v>68</v>
       </c>
       <c r="C70" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -2669,7 +2711,8 @@
         <v>69</v>
       </c>
       <c r="C71" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -2680,7 +2723,8 @@
         <v>70</v>
       </c>
       <c r="C72" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -2691,7 +2735,8 @@
         <v>71</v>
       </c>
       <c r="C73" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -2702,7 +2747,8 @@
         <v>72</v>
       </c>
       <c r="C74" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -2713,7 +2759,8 @@
         <v>73</v>
       </c>
       <c r="C75" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -2724,7 +2771,8 @@
         <v>74</v>
       </c>
       <c r="C76" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -2735,7 +2783,8 @@
         <v>75</v>
       </c>
       <c r="C77" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -2746,7 +2795,8 @@
         <v>76</v>
       </c>
       <c r="C78" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -2757,7 +2807,8 @@
         <v>77</v>
       </c>
       <c r="C79" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -2768,7 +2819,8 @@
         <v>78</v>
       </c>
       <c r="C80" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -2779,7 +2831,8 @@
         <v>79</v>
       </c>
       <c r="C81" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -2790,7 +2843,8 @@
         <v>80</v>
       </c>
       <c r="C82" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -2801,7 +2855,8 @@
         <v>81</v>
       </c>
       <c r="C83" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -2812,7 +2867,8 @@
         <v>82</v>
       </c>
       <c r="C84" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -2823,7 +2879,8 @@
         <v>83</v>
       </c>
       <c r="C85" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -2834,7 +2891,8 @@
         <v>84</v>
       </c>
       <c r="C86" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -2845,7 +2903,8 @@
         <v>85</v>
       </c>
       <c r="C87" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -2856,7 +2915,8 @@
         <v>86</v>
       </c>
       <c r="C88" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -2867,7 +2927,8 @@
         <v>87</v>
       </c>
       <c r="C89" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -2878,7 +2939,8 @@
         <v>88</v>
       </c>
       <c r="C90" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -2889,7 +2951,8 @@
         <v>89</v>
       </c>
       <c r="C91" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -2900,7 +2963,8 @@
         <v>90</v>
       </c>
       <c r="C92" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -2911,7 +2975,8 @@
         <v>91</v>
       </c>
       <c r="C93" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -2922,7 +2987,8 @@
         <v>92</v>
       </c>
       <c r="C94" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -2933,7 +2999,8 @@
         <v>93</v>
       </c>
       <c r="C95" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -2944,7 +3011,8 @@
         <v>94</v>
       </c>
       <c r="C96" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -2955,7 +3023,8 @@
         <v>95</v>
       </c>
       <c r="C97" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -2966,7 +3035,8 @@
         <v>96</v>
       </c>
       <c r="C98" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -2977,7 +3047,8 @@
         <v>97</v>
       </c>
       <c r="C99" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -2988,7 +3059,8 @@
         <v>98</v>
       </c>
       <c r="C100" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -2999,7 +3071,8 @@
         <v>99</v>
       </c>
       <c r="C101" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -3010,7 +3083,8 @@
         <v>100</v>
       </c>
       <c r="C102" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -3021,7 +3095,8 @@
         <v>101</v>
       </c>
       <c r="C103" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -3032,7 +3107,8 @@
         <v>102</v>
       </c>
       <c r="C104" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -3043,7 +3119,8 @@
         <v>103</v>
       </c>
       <c r="C105" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -3054,7 +3131,8 @@
         <v>104</v>
       </c>
       <c r="C106" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -3065,7 +3143,8 @@
         <v>105</v>
       </c>
       <c r="C107" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -3076,7 +3155,8 @@
         <v>106</v>
       </c>
       <c r="C108" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -3087,7 +3167,8 @@
         <v>107</v>
       </c>
       <c r="C109" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -3098,7 +3179,8 @@
         <v>108</v>
       </c>
       <c r="C110" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -3109,7 +3191,8 @@
         <v>109</v>
       </c>
       <c r="C111" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -3120,7 +3203,8 @@
         <v>110</v>
       </c>
       <c r="C112" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -3131,7 +3215,8 @@
         <v>111</v>
       </c>
       <c r="C113" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -3142,7 +3227,8 @@
         <v>112</v>
       </c>
       <c r="C114" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -3153,7 +3239,8 @@
         <v>113</v>
       </c>
       <c r="C115" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -3164,7 +3251,8 @@
         <v>114</v>
       </c>
       <c r="C116" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -3175,7 +3263,8 @@
         <v>115</v>
       </c>
       <c r="C117" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -3186,7 +3275,8 @@
         <v>116</v>
       </c>
       <c r="C118" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -3197,7 +3287,8 @@
         <v>117</v>
       </c>
       <c r="C119" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -3208,7 +3299,8 @@
         <v>118</v>
       </c>
       <c r="C120" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -3219,7 +3311,8 @@
         <v>119</v>
       </c>
       <c r="C121" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.48625999999999997</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -3230,7 +3323,8 @@
         <v>120</v>
       </c>
       <c r="C122" s="38">
-        <v>0.59299999999999997</v>
+        <f t="shared" ref="C122" si="4">0.593*0.82</f>
+        <v>0.48625999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -3243,8 +3337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3554,8 +3648,8 @@
         <v>25</v>
       </c>
       <c r="C27" s="38">
-        <f>prevalence2018!C27/2</f>
-        <v>0.1055</v>
+        <f>prevalence2018!C27/6</f>
+        <v>2.8836666666666663E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3566,8 +3660,8 @@
         <v>26</v>
       </c>
       <c r="C28" s="38">
-        <f>prevalence2018!C28/2</f>
-        <v>0.1055</v>
+        <f>prevalence2018!C28/6</f>
+        <v>2.8836666666666663E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3578,8 +3672,8 @@
         <v>27</v>
       </c>
       <c r="C29" s="38">
-        <f>prevalence2018!C29/2</f>
-        <v>0.1055</v>
+        <f>prevalence2018!C29/6</f>
+        <v>2.8836666666666663E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3590,8 +3684,8 @@
         <v>28</v>
       </c>
       <c r="C30" s="38">
-        <f>prevalence2018!C30/2</f>
-        <v>0.1055</v>
+        <f>prevalence2018!C30/6</f>
+        <v>2.8836666666666663E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -3602,8 +3696,8 @@
         <v>29</v>
       </c>
       <c r="C31" s="38">
-        <f>prevalence2018!C31/2</f>
-        <v>0.1055</v>
+        <f>prevalence2018!C31/6</f>
+        <v>2.8836666666666663E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -3614,8 +3708,8 @@
         <v>30</v>
       </c>
       <c r="C32" s="38">
-        <f>prevalence2018!C32/2</f>
-        <v>0.1055</v>
+        <f>prevalence2018!C32/6</f>
+        <v>2.8836666666666663E-2</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -3626,8 +3720,8 @@
         <v>31</v>
       </c>
       <c r="C33" s="38">
-        <f>prevalence2018!C33/2</f>
-        <v>0.1055</v>
+        <f>prevalence2018!C33/6</f>
+        <v>2.8836666666666663E-2</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -3638,8 +3732,8 @@
         <v>32</v>
       </c>
       <c r="C34" s="38">
-        <f>prevalence2018!C34/2</f>
-        <v>0.1055</v>
+        <f>prevalence2018!C34/6</f>
+        <v>2.8836666666666663E-2</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -3650,8 +3744,8 @@
         <v>33</v>
       </c>
       <c r="C35" s="38">
-        <f>prevalence2018!C35/2</f>
-        <v>0.1055</v>
+        <f>prevalence2018!C35/6</f>
+        <v>2.8836666666666663E-2</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -3662,8 +3756,8 @@
         <v>34</v>
       </c>
       <c r="C36" s="38">
-        <f>prevalence2018!C36/2</f>
-        <v>0.1055</v>
+        <f>prevalence2018!C36/6</f>
+        <v>2.8836666666666663E-2</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -3674,8 +3768,8 @@
         <v>35</v>
       </c>
       <c r="C37" s="38">
-        <f>prevalence2018!C37/2</f>
-        <v>0.157</v>
+        <f>prevalence2018!C37/6</f>
+        <v>4.2390000000000004E-2</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -3686,8 +3780,8 @@
         <v>36</v>
       </c>
       <c r="C38" s="38">
-        <f>prevalence2018!C38/2</f>
-        <v>0.157</v>
+        <f>prevalence2018!C38/6</f>
+        <v>4.2390000000000004E-2</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -3698,8 +3792,8 @@
         <v>37</v>
       </c>
       <c r="C39" s="38">
-        <f>prevalence2018!C39/2</f>
-        <v>0.157</v>
+        <f>prevalence2018!C39/6</f>
+        <v>4.2390000000000004E-2</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -3710,8 +3804,8 @@
         <v>38</v>
       </c>
       <c r="C40" s="38">
-        <f>prevalence2018!C40/2</f>
-        <v>0.157</v>
+        <f>prevalence2018!C40/6</f>
+        <v>4.2390000000000004E-2</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -3722,8 +3816,8 @@
         <v>39</v>
       </c>
       <c r="C41" s="38">
-        <f>prevalence2018!C41/2</f>
-        <v>0.157</v>
+        <f>prevalence2018!C41/6</f>
+        <v>4.2390000000000004E-2</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -3734,8 +3828,8 @@
         <v>40</v>
       </c>
       <c r="C42" s="38">
-        <f>prevalence2018!C42/2</f>
-        <v>0.157</v>
+        <f>prevalence2018!C42/6</f>
+        <v>4.2390000000000004E-2</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -3746,8 +3840,8 @@
         <v>41</v>
       </c>
       <c r="C43" s="38">
-        <f>prevalence2018!C43/2</f>
-        <v>0.157</v>
+        <f>prevalence2018!C43/6</f>
+        <v>4.2390000000000004E-2</v>
       </c>
       <c r="I43" t="s">
         <v>60</v>
@@ -3761,8 +3855,8 @@
         <v>42</v>
       </c>
       <c r="C44" s="38">
-        <f>prevalence2018!C44/2</f>
-        <v>0.157</v>
+        <f>prevalence2018!C44/6</f>
+        <v>4.2390000000000004E-2</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -3773,8 +3867,8 @@
         <v>43</v>
       </c>
       <c r="C45" s="38">
-        <f>prevalence2018!C45/2</f>
-        <v>0.157</v>
+        <f>prevalence2018!C45/6</f>
+        <v>4.2390000000000004E-2</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -3785,8 +3879,8 @@
         <v>44</v>
       </c>
       <c r="C46" s="38">
-        <f>prevalence2018!C46/2</f>
-        <v>0.157</v>
+        <f>prevalence2018!C46/6</f>
+        <v>4.2390000000000004E-2</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -3797,8 +3891,8 @@
         <v>45</v>
       </c>
       <c r="C47" s="38">
-        <f>prevalence2018!C47/2</f>
-        <v>0.2145</v>
+        <f>prevalence2018!C47/6</f>
+        <v>5.8629999999999995E-2</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -3809,8 +3903,8 @@
         <v>46</v>
       </c>
       <c r="C48" s="38">
-        <f>prevalence2018!C48/2</f>
-        <v>0.2145</v>
+        <f>prevalence2018!C48/6</f>
+        <v>5.8629999999999995E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -3821,8 +3915,8 @@
         <v>47</v>
       </c>
       <c r="C49" s="38">
-        <f>prevalence2018!C49/2</f>
-        <v>0.2145</v>
+        <f>prevalence2018!C49/6</f>
+        <v>5.8629999999999995E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -3833,8 +3927,8 @@
         <v>48</v>
       </c>
       <c r="C50" s="38">
-        <f>prevalence2018!C50/2</f>
-        <v>0.2145</v>
+        <f>prevalence2018!C50/6</f>
+        <v>5.8629999999999995E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -3845,8 +3939,8 @@
         <v>49</v>
       </c>
       <c r="C51" s="38">
-        <f>prevalence2018!C51/2</f>
-        <v>0.2145</v>
+        <f>prevalence2018!C51/6</f>
+        <v>5.8629999999999995E-2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -3857,8 +3951,8 @@
         <v>50</v>
       </c>
       <c r="C52" s="38">
-        <f>prevalence2018!C52/2</f>
-        <v>0.2145</v>
+        <f>prevalence2018!C52/6</f>
+        <v>5.8629999999999995E-2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -3869,8 +3963,8 @@
         <v>51</v>
       </c>
       <c r="C53" s="38">
-        <f>prevalence2018!C53/2</f>
-        <v>0.2145</v>
+        <f>prevalence2018!C53/6</f>
+        <v>5.8629999999999995E-2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -3881,8 +3975,8 @@
         <v>52</v>
       </c>
       <c r="C54" s="38">
-        <f>prevalence2018!C54/2</f>
-        <v>0.2145</v>
+        <f>prevalence2018!C54/6</f>
+        <v>5.8629999999999995E-2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -3893,8 +3987,8 @@
         <v>53</v>
       </c>
       <c r="C55" s="38">
-        <f>prevalence2018!C55/2</f>
-        <v>0.2145</v>
+        <f>prevalence2018!C55/6</f>
+        <v>5.8629999999999995E-2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -3905,8 +3999,8 @@
         <v>54</v>
       </c>
       <c r="C56" s="38">
-        <f>prevalence2018!C56/2</f>
-        <v>0.2145</v>
+        <f>prevalence2018!C56/6</f>
+        <v>5.8629999999999995E-2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -3917,8 +4011,8 @@
         <v>55</v>
       </c>
       <c r="C57" s="38">
-        <f>prevalence2018!C57/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C57/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -3929,8 +4023,8 @@
         <v>56</v>
       </c>
       <c r="C58" s="38">
-        <f>prevalence2018!C58/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C58/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -3941,8 +4035,8 @@
         <v>57</v>
       </c>
       <c r="C59" s="38">
-        <f>prevalence2018!C59/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C59/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -3953,8 +4047,8 @@
         <v>58</v>
       </c>
       <c r="C60" s="38">
-        <f>prevalence2018!C60/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C60/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -3965,8 +4059,8 @@
         <v>59</v>
       </c>
       <c r="C61" s="38">
-        <f>prevalence2018!C61/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C61/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -3977,8 +4071,8 @@
         <v>60</v>
       </c>
       <c r="C62" s="38">
-        <f>prevalence2018!C62/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C62/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -3989,8 +4083,8 @@
         <v>61</v>
       </c>
       <c r="C63" s="38">
-        <f>prevalence2018!C63/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C63/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -4001,8 +4095,8 @@
         <v>62</v>
       </c>
       <c r="C64" s="38">
-        <f>prevalence2018!C64/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C64/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -4013,8 +4107,8 @@
         <v>63</v>
       </c>
       <c r="C65" s="38">
-        <f>prevalence2018!C65/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C65/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -4025,8 +4119,8 @@
         <v>64</v>
       </c>
       <c r="C66" s="38">
-        <f>prevalence2018!C66/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C66/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -4037,8 +4131,8 @@
         <v>65</v>
       </c>
       <c r="C67" s="38">
-        <f>prevalence2018!C67/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C67/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -4049,8 +4143,8 @@
         <v>66</v>
       </c>
       <c r="C68" s="38">
-        <f>prevalence2018!C68/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C68/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -4061,8 +4155,8 @@
         <v>67</v>
       </c>
       <c r="C69" s="38">
-        <f>prevalence2018!C69/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C69/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -4073,8 +4167,8 @@
         <v>68</v>
       </c>
       <c r="C70" s="38">
-        <f>prevalence2018!C70/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C70/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -4085,8 +4179,8 @@
         <v>69</v>
       </c>
       <c r="C71" s="38">
-        <f>prevalence2018!C71/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C71/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -4097,8 +4191,8 @@
         <v>70</v>
       </c>
       <c r="C72" s="38">
-        <f>prevalence2018!C72/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C72/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -4109,8 +4203,8 @@
         <v>71</v>
       </c>
       <c r="C73" s="38">
-        <f>prevalence2018!C73/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C73/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -4121,8 +4215,8 @@
         <v>72</v>
       </c>
       <c r="C74" s="38">
-        <f>prevalence2018!C74/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C74/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -4133,8 +4227,8 @@
         <v>73</v>
       </c>
       <c r="C75" s="38">
-        <f>prevalence2018!C75/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C75/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -4145,8 +4239,8 @@
         <v>74</v>
       </c>
       <c r="C76" s="38">
-        <f>prevalence2018!C76/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C76/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -4157,8 +4251,8 @@
         <v>75</v>
       </c>
       <c r="C77" s="38">
-        <f>prevalence2018!C77/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C77/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -4169,8 +4263,8 @@
         <v>76</v>
       </c>
       <c r="C78" s="38">
-        <f>prevalence2018!C78/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C78/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -4181,8 +4275,8 @@
         <v>77</v>
       </c>
       <c r="C79" s="38">
-        <f>prevalence2018!C79/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C79/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -4193,8 +4287,8 @@
         <v>78</v>
       </c>
       <c r="C80" s="38">
-        <f>prevalence2018!C80/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C80/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -4205,8 +4299,8 @@
         <v>79</v>
       </c>
       <c r="C81" s="38">
-        <f>prevalence2018!C81/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C81/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -4217,8 +4311,8 @@
         <v>80</v>
       </c>
       <c r="C82" s="38">
-        <f>prevalence2018!C82/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C82/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -4229,8 +4323,8 @@
         <v>81</v>
       </c>
       <c r="C83" s="38">
-        <f>prevalence2018!C83/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C83/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -4241,8 +4335,8 @@
         <v>82</v>
       </c>
       <c r="C84" s="38">
-        <f>prevalence2018!C84/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C84/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -4253,8 +4347,8 @@
         <v>83</v>
       </c>
       <c r="C85" s="38">
-        <f>prevalence2018!C85/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C85/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -4265,8 +4359,8 @@
         <v>84</v>
       </c>
       <c r="C86" s="38">
-        <f>prevalence2018!C86/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C86/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -4277,8 +4371,8 @@
         <v>85</v>
       </c>
       <c r="C87" s="38">
-        <f>prevalence2018!C87/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C87/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -4289,8 +4383,8 @@
         <v>86</v>
       </c>
       <c r="C88" s="38">
-        <f>prevalence2018!C88/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C88/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -4301,8 +4395,8 @@
         <v>87</v>
       </c>
       <c r="C89" s="38">
-        <f>prevalence2018!C89/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C89/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -4313,8 +4407,8 @@
         <v>88</v>
       </c>
       <c r="C90" s="38">
-        <f>prevalence2018!C90/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C90/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -4325,8 +4419,8 @@
         <v>89</v>
       </c>
       <c r="C91" s="38">
-        <f>prevalence2018!C91/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C91/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -4337,8 +4431,8 @@
         <v>90</v>
       </c>
       <c r="C92" s="38">
-        <f>prevalence2018!C92/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C92/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -4349,8 +4443,8 @@
         <v>91</v>
       </c>
       <c r="C93" s="38">
-        <f>prevalence2018!C93/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C93/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -4361,8 +4455,8 @@
         <v>92</v>
       </c>
       <c r="C94" s="38">
-        <f>prevalence2018!C94/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C94/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -4373,8 +4467,8 @@
         <v>93</v>
       </c>
       <c r="C95" s="38">
-        <f>prevalence2018!C95/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C95/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -4385,8 +4479,8 @@
         <v>94</v>
       </c>
       <c r="C96" s="38">
-        <f>prevalence2018!C96/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C96/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -4397,8 +4491,8 @@
         <v>95</v>
       </c>
       <c r="C97" s="38">
-        <f>prevalence2018!C97/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C97/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -4409,8 +4503,8 @@
         <v>96</v>
       </c>
       <c r="C98" s="38">
-        <f>prevalence2018!C98/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C98/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -4421,8 +4515,8 @@
         <v>97</v>
       </c>
       <c r="C99" s="38">
-        <f>prevalence2018!C99/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C99/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -4433,8 +4527,8 @@
         <v>98</v>
       </c>
       <c r="C100" s="38">
-        <f>prevalence2018!C100/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C100/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -4445,8 +4539,8 @@
         <v>99</v>
       </c>
       <c r="C101" s="38">
-        <f>prevalence2018!C101/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C101/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -4457,8 +4551,8 @@
         <v>100</v>
       </c>
       <c r="C102" s="38">
-        <f>prevalence2018!C102/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C102/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -4469,8 +4563,8 @@
         <v>101</v>
       </c>
       <c r="C103" s="38">
-        <f>prevalence2018!C103/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C103/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -4481,8 +4575,8 @@
         <v>102</v>
       </c>
       <c r="C104" s="38">
-        <f>prevalence2018!C104/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C104/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -4493,8 +4587,8 @@
         <v>103</v>
       </c>
       <c r="C105" s="38">
-        <f>prevalence2018!C105/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C105/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -4505,8 +4599,8 @@
         <v>104</v>
       </c>
       <c r="C106" s="38">
-        <f>prevalence2018!C106/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C106/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -4517,8 +4611,8 @@
         <v>105</v>
       </c>
       <c r="C107" s="38">
-        <f>prevalence2018!C107/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C107/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -4529,8 +4623,8 @@
         <v>106</v>
       </c>
       <c r="C108" s="38">
-        <f>prevalence2018!C108/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C108/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -4541,8 +4635,8 @@
         <v>107</v>
       </c>
       <c r="C109" s="38">
-        <f>prevalence2018!C109/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C109/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -4553,8 +4647,8 @@
         <v>108</v>
       </c>
       <c r="C110" s="38">
-        <f>prevalence2018!C110/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C110/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -4565,8 +4659,8 @@
         <v>109</v>
       </c>
       <c r="C111" s="38">
-        <f>prevalence2018!C111/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C111/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -4577,8 +4671,8 @@
         <v>110</v>
       </c>
       <c r="C112" s="38">
-        <f>prevalence2018!C112/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C112/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -4589,8 +4683,8 @@
         <v>111</v>
       </c>
       <c r="C113" s="38">
-        <f>prevalence2018!C113/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C113/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -4601,8 +4695,8 @@
         <v>112</v>
       </c>
       <c r="C114" s="38">
-        <f>prevalence2018!C114/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C114/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -4613,8 +4707,8 @@
         <v>113</v>
       </c>
       <c r="C115" s="38">
-        <f>prevalence2018!C115/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C115/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -4625,8 +4719,8 @@
         <v>114</v>
       </c>
       <c r="C116" s="38">
-        <f>prevalence2018!C116/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C116/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -4637,8 +4731,8 @@
         <v>115</v>
       </c>
       <c r="C117" s="38">
-        <f>prevalence2018!C117/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C117/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -4649,8 +4743,8 @@
         <v>116</v>
       </c>
       <c r="C118" s="38">
-        <f>prevalence2018!C118/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C118/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -4661,8 +4755,8 @@
         <v>117</v>
       </c>
       <c r="C119" s="38">
-        <f>prevalence2018!C119/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C119/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -4673,8 +4767,8 @@
         <v>118</v>
       </c>
       <c r="C120" s="38">
-        <f>prevalence2018!C120/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C120/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -4685,8 +4779,8 @@
         <v>119</v>
       </c>
       <c r="C121" s="38">
-        <f>prevalence2018!C121/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C121/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -4697,8 +4791,8 @@
         <v>120</v>
       </c>
       <c r="C122" s="38">
-        <f>prevalence2018!C122/2</f>
-        <v>0.29649999999999999</v>
+        <f>prevalence2018!C122/6</f>
+        <v>8.1043333333333328E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incidence of HT is (nearly) correct
To Do:
1. Check final incidence change in run
3. Check risk factors
4. Run test file
5. Log and plot
6. Read in 95% CI for plot
7. Trial outreach campaign
8. Trial HSI event
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_HT.xlsx
+++ b/resources/ResourceFile_Method_HT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/Dropbox/Projects - ongoing/Malawi Project/Thanzi la Onse/04 - Methods Repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CC8026-A282-A54B-9975-77FD01E66026}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2AACFA-32BF-5A40-A6D9-7B4A60711A8B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="15860" tabRatio="723" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4940" yWindow="460" windowWidth="25600" windowHeight="26720" tabRatio="723" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3337,8 +3339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:C122"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3768,8 +3770,8 @@
         <v>35</v>
       </c>
       <c r="C37" s="38">
-        <f>prevalence2018!C37/6</f>
-        <v>4.2390000000000004E-2</v>
+        <f>prevalence2018!C37/12</f>
+        <v>2.1195000000000002E-2</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -3780,8 +3782,8 @@
         <v>36</v>
       </c>
       <c r="C38" s="38">
-        <f>prevalence2018!C38/6</f>
-        <v>4.2390000000000004E-2</v>
+        <f>prevalence2018!C38/12</f>
+        <v>2.1195000000000002E-2</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -3792,8 +3794,8 @@
         <v>37</v>
       </c>
       <c r="C39" s="38">
-        <f>prevalence2018!C39/6</f>
-        <v>4.2390000000000004E-2</v>
+        <f>prevalence2018!C39/12</f>
+        <v>2.1195000000000002E-2</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -3804,8 +3806,8 @@
         <v>38</v>
       </c>
       <c r="C40" s="38">
-        <f>prevalence2018!C40/6</f>
-        <v>4.2390000000000004E-2</v>
+        <f>prevalence2018!C40/12</f>
+        <v>2.1195000000000002E-2</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -3816,8 +3818,8 @@
         <v>39</v>
       </c>
       <c r="C41" s="38">
-        <f>prevalence2018!C41/6</f>
-        <v>4.2390000000000004E-2</v>
+        <f>prevalence2018!C41/12</f>
+        <v>2.1195000000000002E-2</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -3828,8 +3830,8 @@
         <v>40</v>
       </c>
       <c r="C42" s="38">
-        <f>prevalence2018!C42/6</f>
-        <v>4.2390000000000004E-2</v>
+        <f>prevalence2018!C42/12</f>
+        <v>2.1195000000000002E-2</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -3840,8 +3842,8 @@
         <v>41</v>
       </c>
       <c r="C43" s="38">
-        <f>prevalence2018!C43/6</f>
-        <v>4.2390000000000004E-2</v>
+        <f>prevalence2018!C43/12</f>
+        <v>2.1195000000000002E-2</v>
       </c>
       <c r="I43" t="s">
         <v>60</v>
@@ -3855,8 +3857,8 @@
         <v>42</v>
       </c>
       <c r="C44" s="38">
-        <f>prevalence2018!C44/6</f>
-        <v>4.2390000000000004E-2</v>
+        <f>prevalence2018!C44/12</f>
+        <v>2.1195000000000002E-2</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -3867,8 +3869,8 @@
         <v>43</v>
       </c>
       <c r="C45" s="38">
-        <f>prevalence2018!C45/6</f>
-        <v>4.2390000000000004E-2</v>
+        <f>prevalence2018!C45/12</f>
+        <v>2.1195000000000002E-2</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -3879,8 +3881,8 @@
         <v>44</v>
       </c>
       <c r="C46" s="38">
-        <f>prevalence2018!C46/6</f>
-        <v>4.2390000000000004E-2</v>
+        <f>prevalence2018!C46/12</f>
+        <v>2.1195000000000002E-2</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -3891,8 +3893,8 @@
         <v>45</v>
       </c>
       <c r="C47" s="38">
-        <f>prevalence2018!C47/6</f>
-        <v>5.8629999999999995E-2</v>
+        <f>prevalence2018!C47/11</f>
+        <v>3.1980000000000001E-2</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -3903,8 +3905,8 @@
         <v>46</v>
       </c>
       <c r="C48" s="38">
-        <f>prevalence2018!C48/6</f>
-        <v>5.8629999999999995E-2</v>
+        <f>prevalence2018!C48/11</f>
+        <v>3.1980000000000001E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -3915,8 +3917,8 @@
         <v>47</v>
       </c>
       <c r="C49" s="38">
-        <f>prevalence2018!C49/6</f>
-        <v>5.8629999999999995E-2</v>
+        <f>prevalence2018!C49/11</f>
+        <v>3.1980000000000001E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -3927,8 +3929,8 @@
         <v>48</v>
       </c>
       <c r="C50" s="38">
-        <f>prevalence2018!C50/6</f>
-        <v>5.8629999999999995E-2</v>
+        <f>prevalence2018!C50/11</f>
+        <v>3.1980000000000001E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -3939,8 +3941,8 @@
         <v>49</v>
       </c>
       <c r="C51" s="38">
-        <f>prevalence2018!C51/6</f>
-        <v>5.8629999999999995E-2</v>
+        <f>prevalence2018!C51/11</f>
+        <v>3.1980000000000001E-2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -3951,8 +3953,8 @@
         <v>50</v>
       </c>
       <c r="C52" s="38">
-        <f>prevalence2018!C52/6</f>
-        <v>5.8629999999999995E-2</v>
+        <f>prevalence2018!C52/11</f>
+        <v>3.1980000000000001E-2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -3963,8 +3965,8 @@
         <v>51</v>
       </c>
       <c r="C53" s="38">
-        <f>prevalence2018!C53/6</f>
-        <v>5.8629999999999995E-2</v>
+        <f>prevalence2018!C53/11</f>
+        <v>3.1980000000000001E-2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -3975,8 +3977,8 @@
         <v>52</v>
       </c>
       <c r="C54" s="38">
-        <f>prevalence2018!C54/6</f>
-        <v>5.8629999999999995E-2</v>
+        <f>prevalence2018!C54/11</f>
+        <v>3.1980000000000001E-2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -3987,8 +3989,8 @@
         <v>53</v>
       </c>
       <c r="C55" s="38">
-        <f>prevalence2018!C55/6</f>
-        <v>5.8629999999999995E-2</v>
+        <f>prevalence2018!C55/11</f>
+        <v>3.1980000000000001E-2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -3999,8 +4001,8 @@
         <v>54</v>
       </c>
       <c r="C56" s="38">
-        <f>prevalence2018!C56/6</f>
-        <v>5.8629999999999995E-2</v>
+        <f>prevalence2018!C56/11</f>
+        <v>3.1980000000000001E-2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -4011,8 +4013,8 @@
         <v>55</v>
       </c>
       <c r="C57" s="38">
-        <f>prevalence2018!C57/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C57/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -4023,8 +4025,8 @@
         <v>56</v>
       </c>
       <c r="C58" s="38">
-        <f>prevalence2018!C58/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C58/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -4035,8 +4037,8 @@
         <v>57</v>
       </c>
       <c r="C59" s="38">
-        <f>prevalence2018!C59/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C59/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -4047,8 +4049,8 @@
         <v>58</v>
       </c>
       <c r="C60" s="38">
-        <f>prevalence2018!C60/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C60/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -4059,8 +4061,8 @@
         <v>59</v>
       </c>
       <c r="C61" s="38">
-        <f>prevalence2018!C61/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C61/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -4071,8 +4073,8 @@
         <v>60</v>
       </c>
       <c r="C62" s="38">
-        <f>prevalence2018!C62/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C62/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -4083,8 +4085,8 @@
         <v>61</v>
       </c>
       <c r="C63" s="38">
-        <f>prevalence2018!C63/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C63/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -4095,8 +4097,8 @@
         <v>62</v>
       </c>
       <c r="C64" s="38">
-        <f>prevalence2018!C64/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C64/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -4107,8 +4109,8 @@
         <v>63</v>
       </c>
       <c r="C65" s="38">
-        <f>prevalence2018!C65/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C65/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -4119,8 +4121,8 @@
         <v>64</v>
       </c>
       <c r="C66" s="38">
-        <f>prevalence2018!C66/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C66/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -4131,8 +4133,8 @@
         <v>65</v>
       </c>
       <c r="C67" s="38">
-        <f>prevalence2018!C67/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C67/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -4143,8 +4145,8 @@
         <v>66</v>
       </c>
       <c r="C68" s="38">
-        <f>prevalence2018!C68/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C68/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -4155,8 +4157,8 @@
         <v>67</v>
       </c>
       <c r="C69" s="38">
-        <f>prevalence2018!C69/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C69/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -4167,8 +4169,8 @@
         <v>68</v>
       </c>
       <c r="C70" s="38">
-        <f>prevalence2018!C70/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C70/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -4179,8 +4181,8 @@
         <v>69</v>
       </c>
       <c r="C71" s="38">
-        <f>prevalence2018!C71/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C71/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -4191,8 +4193,8 @@
         <v>70</v>
       </c>
       <c r="C72" s="38">
-        <f>prevalence2018!C72/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C72/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -4203,8 +4205,8 @@
         <v>71</v>
       </c>
       <c r="C73" s="38">
-        <f>prevalence2018!C73/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C73/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -4215,8 +4217,8 @@
         <v>72</v>
       </c>
       <c r="C74" s="38">
-        <f>prevalence2018!C74/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C74/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -4227,8 +4229,8 @@
         <v>73</v>
       </c>
       <c r="C75" s="38">
-        <f>prevalence2018!C75/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C75/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -4239,8 +4241,8 @@
         <v>74</v>
       </c>
       <c r="C76" s="38">
-        <f>prevalence2018!C76/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C76/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -4251,8 +4253,8 @@
         <v>75</v>
       </c>
       <c r="C77" s="38">
-        <f>prevalence2018!C77/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C77/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -4263,8 +4265,8 @@
         <v>76</v>
       </c>
       <c r="C78" s="38">
-        <f>prevalence2018!C78/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C78/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -4275,8 +4277,8 @@
         <v>77</v>
       </c>
       <c r="C79" s="38">
-        <f>prevalence2018!C79/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C79/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -4287,8 +4289,8 @@
         <v>78</v>
       </c>
       <c r="C80" s="38">
-        <f>prevalence2018!C80/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C80/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -4299,8 +4301,8 @@
         <v>79</v>
       </c>
       <c r="C81" s="38">
-        <f>prevalence2018!C81/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C81/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -4311,8 +4313,8 @@
         <v>80</v>
       </c>
       <c r="C82" s="38">
-        <f>prevalence2018!C82/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C82/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -4323,8 +4325,8 @@
         <v>81</v>
       </c>
       <c r="C83" s="38">
-        <f>prevalence2018!C83/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C83/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -4335,8 +4337,8 @@
         <v>82</v>
       </c>
       <c r="C84" s="38">
-        <f>prevalence2018!C84/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C84/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -4347,8 +4349,8 @@
         <v>83</v>
       </c>
       <c r="C85" s="38">
-        <f>prevalence2018!C85/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C85/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -4359,8 +4361,8 @@
         <v>84</v>
       </c>
       <c r="C86" s="38">
-        <f>prevalence2018!C86/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C86/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -4371,8 +4373,8 @@
         <v>85</v>
       </c>
       <c r="C87" s="38">
-        <f>prevalence2018!C87/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C87/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -4383,8 +4385,8 @@
         <v>86</v>
       </c>
       <c r="C88" s="38">
-        <f>prevalence2018!C88/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C88/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -4395,8 +4397,8 @@
         <v>87</v>
       </c>
       <c r="C89" s="38">
-        <f>prevalence2018!C89/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C89/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -4407,8 +4409,8 @@
         <v>88</v>
       </c>
       <c r="C90" s="38">
-        <f>prevalence2018!C90/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C90/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -4419,8 +4421,8 @@
         <v>89</v>
       </c>
       <c r="C91" s="38">
-        <f>prevalence2018!C91/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C91/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -4431,8 +4433,8 @@
         <v>90</v>
       </c>
       <c r="C92" s="38">
-        <f>prevalence2018!C92/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C92/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -4443,8 +4445,8 @@
         <v>91</v>
       </c>
       <c r="C93" s="38">
-        <f>prevalence2018!C93/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C93/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -4455,8 +4457,8 @@
         <v>92</v>
       </c>
       <c r="C94" s="38">
-        <f>prevalence2018!C94/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C94/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -4467,8 +4469,8 @@
         <v>93</v>
       </c>
       <c r="C95" s="38">
-        <f>prevalence2018!C95/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C95/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -4479,8 +4481,8 @@
         <v>94</v>
       </c>
       <c r="C96" s="38">
-        <f>prevalence2018!C96/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C96/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -4491,8 +4493,8 @@
         <v>95</v>
       </c>
       <c r="C97" s="38">
-        <f>prevalence2018!C97/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C97/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -4503,8 +4505,8 @@
         <v>96</v>
       </c>
       <c r="C98" s="38">
-        <f>prevalence2018!C98/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C98/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -4515,8 +4517,8 @@
         <v>97</v>
       </c>
       <c r="C99" s="38">
-        <f>prevalence2018!C99/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C99/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -4527,8 +4529,8 @@
         <v>98</v>
       </c>
       <c r="C100" s="38">
-        <f>prevalence2018!C100/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C100/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -4539,8 +4541,8 @@
         <v>99</v>
       </c>
       <c r="C101" s="38">
-        <f>prevalence2018!C101/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C101/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -4551,8 +4553,8 @@
         <v>100</v>
       </c>
       <c r="C102" s="38">
-        <f>prevalence2018!C102/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C102/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -4563,8 +4565,8 @@
         <v>101</v>
       </c>
       <c r="C103" s="38">
-        <f>prevalence2018!C103/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C103/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -4575,8 +4577,8 @@
         <v>102</v>
       </c>
       <c r="C104" s="38">
-        <f>prevalence2018!C104/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C104/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -4587,8 +4589,8 @@
         <v>103</v>
       </c>
       <c r="C105" s="38">
-        <f>prevalence2018!C105/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C105/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -4599,8 +4601,8 @@
         <v>104</v>
       </c>
       <c r="C106" s="38">
-        <f>prevalence2018!C106/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C106/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -4611,8 +4613,8 @@
         <v>105</v>
       </c>
       <c r="C107" s="38">
-        <f>prevalence2018!C107/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C107/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -4623,8 +4625,8 @@
         <v>106</v>
       </c>
       <c r="C108" s="38">
-        <f>prevalence2018!C108/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C108/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -4635,8 +4637,8 @@
         <v>107</v>
       </c>
       <c r="C109" s="38">
-        <f>prevalence2018!C109/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C109/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -4647,8 +4649,8 @@
         <v>108</v>
       </c>
       <c r="C110" s="38">
-        <f>prevalence2018!C110/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C110/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -4659,8 +4661,8 @@
         <v>109</v>
       </c>
       <c r="C111" s="38">
-        <f>prevalence2018!C111/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C111/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -4671,8 +4673,8 @@
         <v>110</v>
       </c>
       <c r="C112" s="38">
-        <f>prevalence2018!C112/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C112/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -4683,8 +4685,8 @@
         <v>111</v>
       </c>
       <c r="C113" s="38">
-        <f>prevalence2018!C113/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C113/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -4695,8 +4697,8 @@
         <v>112</v>
       </c>
       <c r="C114" s="38">
-        <f>prevalence2018!C114/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C114/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -4707,8 +4709,8 @@
         <v>113</v>
       </c>
       <c r="C115" s="38">
-        <f>prevalence2018!C115/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C115/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -4719,8 +4721,8 @@
         <v>114</v>
       </c>
       <c r="C116" s="38">
-        <f>prevalence2018!C116/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C116/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -4731,8 +4733,8 @@
         <v>115</v>
       </c>
       <c r="C117" s="38">
-        <f>prevalence2018!C117/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C117/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -4743,8 +4745,8 @@
         <v>116</v>
       </c>
       <c r="C118" s="38">
-        <f>prevalence2018!C118/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C118/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -4755,8 +4757,8 @@
         <v>117</v>
       </c>
       <c r="C119" s="38">
-        <f>prevalence2018!C119/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C119/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -4767,8 +4769,8 @@
         <v>118</v>
       </c>
       <c r="C120" s="38">
-        <f>prevalence2018!C120/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C120/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -4779,8 +4781,8 @@
         <v>119</v>
       </c>
       <c r="C121" s="38">
-        <f>prevalence2018!C121/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C121/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -4791,8 +4793,8 @@
         <v>120</v>
       </c>
       <c r="C122" s="38">
-        <f>prevalence2018!C122/6</f>
-        <v>8.1043333333333328E-2</v>
+        <f>prevalence2018!C122/12</f>
+        <v>4.0521666666666664E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Address Tim comments. Read in error, continued2
1. Check all variable names to ensure they are self-evident
2. Provide description for each def section\
3. Add :param to comments
4. Excel read in

To do
1. Log and Plot
2. clean up (remove FH)
3. HSI event flesh out HTN
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_HT.xlsx
+++ b/resources/ResourceFile_Method_HT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/Dropbox/Projects - ongoing/Malawi Project/Thanzi la Onse/04 - Methods Repository/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2AACFA-32BF-5A40-A6D9-7B4A60711A8B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11AD58F-4A36-EE44-9703-7D5FA1657419}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="460" windowWidth="25600" windowHeight="26720" tabRatio="723" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16060" tabRatio="723" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -186,9 +184,6 @@
   </si>
   <si>
     <t>probability</t>
-  </si>
-  <si>
-    <t>prob_basic</t>
   </si>
   <si>
     <t>Prevalence/incidence to also depend on lifestyle factors and HIV (where relevant)</t>
@@ -508,9 +503,6 @@
     <t>max</t>
   </si>
   <si>
-    <t>parameter</t>
-  </si>
-  <si>
     <t>value2</t>
   </si>
   <si>
@@ -575,6 +567,12 @@
   </si>
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>parameter_name</t>
+  </si>
+  <si>
+    <t>prob_ht_basic</t>
   </si>
 </sst>
 </file>
@@ -1341,7 +1339,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
@@ -1374,7 +1372,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
@@ -1385,7 +1383,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -1399,7 +1397,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" s="22"/>
       <c r="H14" s="19"/>
@@ -1409,7 +1407,7 @@
         <v>37</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H15" s="19"/>
     </row>
@@ -1427,7 +1425,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H17" s="18"/>
     </row>
@@ -1436,7 +1434,7 @@
         <v>32</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
@@ -1465,7 +1463,7 @@
         <v>35</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="17" x14ac:dyDescent="0.2">
@@ -1473,7 +1471,7 @@
         <v>41</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
@@ -1617,7 +1615,7 @@
         <v>46</v>
       </c>
       <c r="J7" s="41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K7" s="34" t="s">
         <v>30</v>
@@ -1632,10 +1630,10 @@
     </row>
     <row r="8" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I8" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="36" t="s">
         <v>52</v>
-      </c>
-      <c r="J8" s="36" t="s">
-        <v>53</v>
       </c>
       <c r="K8" s="36" t="s">
         <v>30</v>
@@ -1649,10 +1647,10 @@
     </row>
     <row r="9" spans="9:14" ht="34" x14ac:dyDescent="0.2">
       <c r="I9" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J9" s="41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K9" s="36" t="s">
         <v>43</v>
@@ -1666,10 +1664,10 @@
     </row>
     <row r="10" spans="9:14" ht="17" x14ac:dyDescent="0.2">
       <c r="I10" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="J10" s="41" t="s">
         <v>92</v>
-      </c>
-      <c r="J10" s="41" t="s">
-        <v>93</v>
       </c>
       <c r="K10" s="36" t="s">
         <v>43</v>
@@ -1684,16 +1682,16 @@
     <row r="11" spans="9:14" s="26" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="I11" s="27"/>
       <c r="J11" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K11" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L11" s="14" t="s">
         <v>26</v>
       </c>
       <c r="M11" s="40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N11" s="5"/>
     </row>
@@ -1701,13 +1699,13 @@
       <c r="I12" s="39"/>
       <c r="J12" s="41"/>
       <c r="K12" s="36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L12" s="36" t="s">
         <v>26</v>
       </c>
       <c r="M12" s="36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N12" s="16"/>
     </row>
@@ -1742,13 +1740,13 @@
       <c r="I15" s="42"/>
       <c r="J15" s="28"/>
       <c r="K15" s="36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L15" s="36" t="s">
         <v>26</v>
       </c>
       <c r="M15" s="36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N15" s="24"/>
     </row>
@@ -1756,13 +1754,13 @@
       <c r="I16" s="27"/>
       <c r="J16" s="29"/>
       <c r="K16" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L16" s="14" t="s">
         <v>26</v>
       </c>
       <c r="M16" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N16" s="24"/>
     </row>
@@ -1786,19 +1784,19 @@
     </row>
     <row r="20" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I20" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J20" s="26"/>
     </row>
     <row r="21" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I21" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J21" s="26"/>
     </row>
     <row r="22" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I22" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J22" s="26"/>
     </row>
@@ -1810,7 +1808,7 @@
     </row>
     <row r="24" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I24" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J24" s="26"/>
     </row>
@@ -1833,7 +1831,7 @@
     </row>
     <row r="28" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I28" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J28" s="31"/>
       <c r="K28" s="31"/>
@@ -1842,7 +1840,7 @@
     </row>
     <row r="29" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I29" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J29" s="31"/>
       <c r="K29" s="31"/>
@@ -1851,7 +1849,7 @@
     </row>
     <row r="30" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I30" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J30" s="31"/>
       <c r="K30" s="31"/>
@@ -3339,7 +3337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
@@ -3846,7 +3844,7 @@
         <v>2.1195000000000002E-2</v>
       </c>
       <c r="I43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -4806,8 +4804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FFD66BD-C60D-C14A-9E33-3479AADC1850}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4818,39 +4816,39 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="38" t="s">
+      <c r="I1" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="38" t="s">
         <v>106</v>
-      </c>
-      <c r="G1" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="38" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="B2" s="38">
         <v>1</v>
@@ -4864,7 +4862,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="38">
         <v>1.66</v>
@@ -4896,7 +4894,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="38">
         <v>2</v>
@@ -4910,7 +4908,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="38">
         <v>1.65</v>
@@ -4948,27 +4946,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
         <v>98</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>99</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>101</v>
-      </c>
-      <c r="F1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B2">
         <v>25</v>
@@ -4988,7 +4986,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B3">
         <v>25</v>
@@ -5008,7 +5006,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B4">
         <v>25</v>
@@ -5028,7 +5026,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B5">
         <v>25</v>
@@ -5048,7 +5046,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B6">
         <v>35</v>
@@ -5068,7 +5066,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B7">
         <v>45</v>
@@ -5088,7 +5086,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B8">
         <v>55</v>
@@ -5108,7 +5106,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B9">
         <v>25</v>
@@ -5128,7 +5126,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B10">
         <v>35</v>
@@ -5148,7 +5146,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B11">
         <v>45</v>
@@ -5168,7 +5166,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B12">
         <v>55</v>
@@ -5188,7 +5186,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B13">
         <v>25</v>
@@ -5208,7 +5206,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B14">
         <v>35</v>
@@ -5228,7 +5226,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B15">
         <v>45</v>
@@ -5248,7 +5246,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B16">
         <v>55</v>
@@ -5288,17 +5286,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="48" t="s">
         <v>17</v>
@@ -5306,46 +5304,46 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="45" t="s">
-        <v>73</v>
-      </c>
       <c r="C3" s="45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="49" t="s">
-        <v>77</v>
-      </c>
       <c r="C4" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="45" t="s">
-        <v>79</v>
-      </c>
       <c r="C5" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="45" t="s">
-        <v>81</v>
-      </c>
       <c r="C6" s="46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Address Tim comments. Read in fixed - yay. Clean up
1. Check all variable names to ensure they are self-evident
2. Provide description for each def section\
3. Add :param to comments
4. Excel read in

To do
1. Log and Plot
2. clean up (remove FH)
3. HSI event flesh out HTN
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_HT.xlsx
+++ b/resources/ResourceFile_Method_HT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11AD58F-4A36-EE44-9703-7D5FA1657419}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58CFE5E-B3A9-A143-B939-585139BA16B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16060" tabRatio="723" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="125">
   <si>
     <t>Name:</t>
   </si>
@@ -240,9 +240,6 @@
   </si>
   <si>
     <t>prob_htgivendiabetes</t>
-  </si>
-  <si>
-    <t>prob_htgivenfamhis</t>
   </si>
   <si>
     <t>https://github.com/UCL/TLOmodel/tree/feature/msmit-NCDwithHS</t>
@@ -1339,7 +1336,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
@@ -1372,7 +1369,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
@@ -1383,7 +1380,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -1397,7 +1394,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="22"/>
       <c r="H14" s="19"/>
@@ -1407,7 +1404,7 @@
         <v>37</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H15" s="19"/>
     </row>
@@ -1425,7 +1422,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H17" s="18"/>
     </row>
@@ -1434,7 +1431,7 @@
         <v>32</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
@@ -1463,7 +1460,7 @@
         <v>35</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="17" x14ac:dyDescent="0.2">
@@ -1647,10 +1644,10 @@
     </row>
     <row r="9" spans="9:14" ht="34" x14ac:dyDescent="0.2">
       <c r="I9" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J9" s="41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K9" s="36" t="s">
         <v>43</v>
@@ -1664,10 +1661,10 @@
     </row>
     <row r="10" spans="9:14" ht="17" x14ac:dyDescent="0.2">
       <c r="I10" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="41" t="s">
         <v>91</v>
-      </c>
-      <c r="J10" s="41" t="s">
-        <v>92</v>
       </c>
       <c r="K10" s="36" t="s">
         <v>43</v>
@@ -1682,7 +1679,7 @@
     <row r="11" spans="9:14" s="26" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="I11" s="27"/>
       <c r="J11" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K11" s="33" t="s">
         <v>53</v>
@@ -1796,7 +1793,7 @@
     </row>
     <row r="22" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I22" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J22" s="26"/>
     </row>
@@ -4802,10 +4799,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FFD66BD-C60D-C14A-9E33-3479AADC1850}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4816,39 +4813,39 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="D1" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="E1" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="F1" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="I1" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="I1" s="38" t="s">
+      <c r="J1" s="38" t="s">
         <v>105</v>
-      </c>
-      <c r="J1" s="38" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" s="38">
         <v>1</v>
@@ -4904,29 +4901,6 @@
       </c>
       <c r="D4" s="44">
         <v>2.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="38">
-        <v>1.65</v>
-      </c>
-      <c r="C5" s="38">
-        <v>1.3</v>
-      </c>
-      <c r="D5" s="38">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E5" s="38">
-        <v>2.4</v>
-      </c>
-      <c r="F5" s="38">
-        <v>1.8</v>
-      </c>
-      <c r="G5" s="38">
-        <v>3.2</v>
       </c>
     </row>
   </sheetData>
@@ -4946,27 +4920,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
         <v>97</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>98</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>99</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>100</v>
-      </c>
-      <c r="F1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2">
         <v>25</v>
@@ -4986,7 +4960,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3">
         <v>25</v>
@@ -5006,7 +4980,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4">
         <v>25</v>
@@ -5026,7 +5000,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5">
         <v>25</v>
@@ -5046,7 +5020,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6">
         <v>35</v>
@@ -5066,7 +5040,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7">
         <v>45</v>
@@ -5086,7 +5060,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8">
         <v>55</v>
@@ -5106,7 +5080,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9">
         <v>25</v>
@@ -5126,7 +5100,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10">
         <v>35</v>
@@ -5146,7 +5120,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11">
         <v>45</v>
@@ -5166,7 +5140,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12">
         <v>55</v>
@@ -5186,7 +5160,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13">
         <v>25</v>
@@ -5206,7 +5180,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14">
         <v>35</v>
@@ -5226,7 +5200,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15">
         <v>45</v>
@@ -5246,7 +5220,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16">
         <v>55</v>
@@ -5286,17 +5260,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" s="48" t="s">
         <v>17</v>
@@ -5304,46 +5278,46 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="45" t="s">
-        <v>72</v>
-      </c>
       <c r="C3" s="45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="49" t="s">
-        <v>76</v>
-      </c>
       <c r="C4" s="45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="45" t="s">
-        <v>78</v>
-      </c>
       <c r="C5" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="45" t="s">
-        <v>80</v>
-      </c>
       <c r="C6" s="46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Pytest (ask Asif about age/time code)
To Do:
0. Define new groupby for validation
1. Read in BMI csv Stef Excel read in (list)
2. Plot data vs model
3. Add assert HTN>0 and HTN same as data
3. Trial outreach campaign
4. Trial HSI event

Done:
1. Add more descriptions
2. Add Param: info
3. Use groupby
4. Changed naming as per Tim's comments
5. Add 2 logging events
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_HT.xlsx
+++ b/resources/ResourceFile_Method_HT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E7BA42-9BFD-BB42-B58A-2286E70CE1C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055AF3E8-BAA9-FD4F-843D-FE0FA87B999C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16060" tabRatio="723" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4040" yWindow="460" windowWidth="14400" windowHeight="16060" tabRatio="723" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -4777,7 +4779,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Tidy (comment, condense, and flake8) hypertension.py.
To Do:
0. Define new groupby for validation
1. Read in BMI csv Stef Excel read in (list)
2. Plot data vs model
3. Add assert HTN>0 and HTN same as data
3. Trial outreach campaign
4. Trial HSI event

Done:
1. Add more descriptions
2. Add Param: info
3. Use groupby
4. Changed naming as per Tim's comments
5. Add 2 logging events
6. check flake8
7. add more comments
8. move all code to correct place (away from debug code)
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_HT.xlsx
+++ b/resources/ResourceFile_Method_HT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055AF3E8-BAA9-FD4F-843D-FE0FA87B999C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D101CD5E-67E8-3246-B47D-658EE61CA253}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="460" windowWidth="14400" windowHeight="16060" tabRatio="723" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" tabRatio="723" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Additional data comparison for HTN
DONE
1. Tidied up health states and daly weights
2. checked correct daly values are assigned
3. Generated properties for t2dm complications

To Do:
1. upload data on complications
2. Try read in BMI csv Stef Excel read in (list)
3. flake8 redo on additional code
4. Upload Price data for t2dm and htn

Post UCl review
1. Trial outreach campaign
2. Trial HSI event
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_HT.xlsx
+++ b/resources/ResourceFile_Method_HT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17960B69-EC02-894E-B85B-31395B4FFE99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A304D9B-5382-884B-8869-7A8CC7B70EC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" tabRatio="723" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="26720" tabRatio="723" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="124">
   <si>
     <t>Name:</t>
   </si>
@@ -554,6 +554,21 @@
   </si>
   <si>
     <t>prob_ht_basic</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>divala</t>
+  </si>
+  <si>
+    <t>ruecker</t>
+  </si>
+  <si>
+    <t>ramirez</t>
+  </si>
+  <si>
+    <t>ramirez mala</t>
   </si>
 </sst>
 </file>
@@ -1848,7 +1863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C57" sqref="C57:C122"/>
     </sheetView>
   </sheetViews>
@@ -4827,10 +4842,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7146AB7-8FEC-7F45-A5FB-E9FDE5B75DD4}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5153,6 +5168,91 @@
       </c>
       <c r="F16">
         <v>0.67500000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>80</v>
+      </c>
+      <c r="D17">
+        <v>0.15</v>
+      </c>
+      <c r="E17">
+        <v>0.13</v>
+      </c>
+      <c r="F17">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>65</v>
+      </c>
+      <c r="D18">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="E18">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="F18">
+        <v>0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>70</v>
+      </c>
+      <c r="D19">
+        <v>0.252</v>
+      </c>
+      <c r="E19">
+        <v>0.222</v>
+      </c>
+      <c r="F19">
+        <v>0.316</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>90</v>
+      </c>
+      <c r="D20">
+        <v>0.23</v>
+      </c>
+      <c r="E20">
+        <v>0.2</v>
+      </c>
+      <c r="F20">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>